<commit_message>
add Girona-Mata paper 2025
</commit_message>
<xml_diff>
--- a/publications.xlsx
+++ b/publications.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S81"/>
+  <dimension ref="A1:S82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -534,32 +534,36 @@
       <c r="A2" t="inlineStr"/>
       <c r="B2" t="inlineStr">
         <is>
-          <t>L. Uebbing, H. L. Joakimsen, L. T. Luppino, I. Martinsen, A. McDonald, K. K. Wickstr&amp;oslash;m, S. Lef&amp;egrave;vre, A. B. Salberg, S. Hosking, R. Jenssen</t>
+          <t>B. R. Evans, A. Lowe, A. Crawford, A. Fleming, J. S. Hosking</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://openreview.net/forum?id=7TwvcPAyxX</t>
+          <t>10.5194/egusphere-2025-2886</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Northern Lights Deep Learning Conference 2025</t>
+          <t>EGUsphere</t>
         </is>
       </c>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>1--28</t>
+        </is>
+      </c>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr">
         <is>
-          <t>Investigating the Impact of Feature Reduction for Deep Learning-based Seasonal Sea Ice Forecasting</t>
+          <t>Icebergs, jigsaw puzzles and genealogy: Automated multi-generational iceberg tracking and lineage reconstruction</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
@@ -569,13 +573,17 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>https://openreview.net/forum?id=7TwvcPAyxX</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr"/>
+          <t>https://egusphere.copernicus.org/preprints/2025/egusphere-2025-2886/</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>2024</t>
+          <t>2025</t>
         </is>
       </c>
     </row>
@@ -583,36 +591,32 @@
       <c r="A3" t="inlineStr"/>
       <c r="B3" t="inlineStr">
         <is>
-          <t>M. Girona-Mata, A. Orr, M. Widmann, D. Bannister, G. H. Dars, S. Hosking, J. Norris, D. Ocio, T. Phillips, J. Steiner, R. E. Turner</t>
+          <t>L. Uebbing, H. L. Joakimsen, L. T. Luppino, I. Martinsen, A. McDonald, K. K. Wickstr&amp;oslash;m, S. Lef&amp;egrave;vre, A. B. Salberg, S. Hosking, R. Jenssen</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>10.5194/egusphere-2024-2805</t>
+          <t>https://openreview.net/forum?id=7TwvcPAyxX</t>
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>EGUsphere</t>
+          <t>Northern Lights Deep Learning Conference 2025</t>
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>1--33</t>
-        </is>
-      </c>
+      <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr"/>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Probabilistic precipitation downscaling for ungauged mountain sites: a pilot study for the Hindu Kush Karakoram Himalaya</t>
+          <t>Investigating the Impact of Feature Reduction for Deep Learning-based Seasonal Sea Ice Forecasting</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
@@ -622,7 +626,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>https://egusphere.copernicus.org/preprints/2024/egusphere-2024-2805/</t>
+          <t>https://openreview.net/forum?id=7TwvcPAyxX</t>
         </is>
       </c>
       <c r="R3" t="inlineStr"/>
@@ -918,36 +922,32 @@
       <c r="A10" t="inlineStr"/>
       <c r="B10" t="inlineStr">
         <is>
-          <t>E. Bowler, J. Byrne, L.-M. Leclerc, A. Roberto-Charron, M. S. Rogers, R. D. Cavanagh, J. Harasimo, M. L. Lancaster, R. S. Chan, O. Strickson, J. Wilkinson, R. Downie, J. S. Hosking, T. R. Andersson</t>
+          <t>M. Girona-Mata, A. Orr, M. Widmann, D. Bannister, G. H. Dars, S. Hosking, J. Norris, D. Ocio, T. Phillips, J. Steiner, R. E. Turner</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1002/2688-8319.70034</t>
+          <t>10.5194/hess-29-3073-2025</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Ecological Solutions and Evidence</t>
+          <t>Hydrology and Earth System Sciences</t>
         </is>
       </c>
       <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>Phys.org, black, https://phys.org/news/2025-05-ai-tool-aids-caribou-arctic.html; Anadolu Agency, blue, https://www.aa.com.tr/en/environment/new-ai-tool-can-help-protect-migration-routes-of-endangered-caribou-in-arctic-study/3583642; Business Weekly, grey, https://www.businessweekly.co.uk/posts/british-antarctic-survey-puts-ai-into-arctic-to-aid-caribou-conservation; Press Release, HotPink, https://www.bas.ac.uk/media-post/new-ai-tool-aids-caribou-conservation-in-a-changing-arctic/; Canada's National Observer, red, https://www.nationalobserver.com/2025/06/11/news/ai-protect-caribou-migration-changing-arctic</t>
-        </is>
-      </c>
+      <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>14</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>e70034</t>
+          <t>3073--3100</t>
         </is>
       </c>
       <c r="L10" t="inlineStr"/>
@@ -955,7 +955,7 @@
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="inlineStr">
         <is>
-          <t>AI sea ice forecasts for Arctic conservation: A case study predicting the timing of caribou sea ice migrations</t>
+          <t>Probabilistic precipitation downscaling for ungauged mountain sites: a pilot study for the Hindu Kush Himalaya</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
@@ -965,12 +965,12 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>https://besjournals.onlinelibrary.wiley.com/doi/abs/10.1002/2688-8319.70034</t>
+          <t>https://hess.copernicus.org/articles/29/3073/2025/</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>29</t>
         </is>
       </c>
       <c r="S10" t="inlineStr">
@@ -983,28 +983,36 @@
       <c r="A11" t="inlineStr"/>
       <c r="B11" t="inlineStr">
         <is>
-          <t>R. E. Rouse, H. Moss, S. Hosking, A. McRobie, E. Shuckburgh</t>
+          <t>E. Bowler, J. Byrne, L.-M. Leclerc, A. Roberto-Charron, M. S. Rogers, R. D. Cavanagh, J. Harasimo, M. L. Lancaster, R. S. Chan, O. Strickson, J. Wilkinson, R. Downie, J. S. Hosking, T. R. Andersson</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>10.1017/eds.2025.16</t>
+          <t>https://doi.org/10.1002/2688-8319.70034</t>
         </is>
       </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Environmental Data Science</t>
+          <t>Ecological Solutions and Evidence</t>
         </is>
       </c>
       <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Phys.org, black, https://phys.org/news/2025-05-ai-tool-aids-caribou-arctic.html; Anadolu Agency, blue, https://www.aa.com.tr/en/environment/new-ai-tool-can-help-protect-migration-routes-of-endangered-caribou-in-arctic-study/3583642; Business Weekly, grey, https://www.businessweekly.co.uk/posts/british-antarctic-survey-puts-ai-into-arctic-to-aid-caribou-conservation; Press Release, HotPink, https://www.bas.ac.uk/media-post/new-ai-tool-aids-caribou-conservation-in-a-changing-arctic/; Canada's National Observer, red, https://www.nationalobserver.com/2025/06/11/news/ai-protect-caribou-migration-changing-arctic</t>
+        </is>
+      </c>
       <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>e26</t>
+          <t>e70034</t>
         </is>
       </c>
       <c r="L11" t="inlineStr"/>
@@ -1012,7 +1020,7 @@
       <c r="N11" t="inlineStr"/>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Reflective error: a metric for assessing predictive performance at extreme events</t>
+          <t>AI sea ice forecasts for Arctic conservation: A case study predicting the timing of caribou sea ice migrations</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
@@ -1020,10 +1028,14 @@
           <t>article</t>
         </is>
       </c>
-      <c r="Q11" t="inlineStr"/>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>https://besjournals.onlinelibrary.wiley.com/doi/abs/10.1002/2688-8319.70034</t>
+        </is>
+      </c>
       <c r="R11" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6</t>
         </is>
       </c>
       <c r="S11" t="inlineStr">
@@ -1036,36 +1048,36 @@
       <c r="A12" t="inlineStr"/>
       <c r="B12" t="inlineStr">
         <is>
-          <t>A. Allen, S. Markou, W. Tebbutt, J. Requeima, W. P. Bruinsma, T. R. Andersson, N. D. Herzog, M. Chantry, J. S. Hosking, R. E. Turner</t>
+          <t>R. E. Rouse, H. Moss, S. Hosking, A. McRobie, E. Shuckburgh</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1038/s41586-025-08897-0</t>
+          <t>10.1017/eds.2025.16</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Nature</t>
+          <t>Environmental Data Science</t>
         </is>
       </c>
       <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>Guardian, blue, https://www.theguardian.com/technology/2025/mar/20/ai-aardvark-weather-prediction-forecasting-artificial-intelligence; FT, DarkOrange, https://www.ft.com/content/73492128-5822-4bb2-b953-64217eb303e4; New Scientist, grey, https://www.newscientist.com/article/2472659-ai-can-forecast-the-weather-in-seconds-without-needing-supercomputers/; Independent, red, https://www.independent.co.uk/tech/ai-weather-forecast-aardvark-cambridge-b2717122.html; Blog, black, https://www.turing.ac.uk/blog/project-aardvark-reimagining-ai-weather-prediction</t>
-        </is>
-      </c>
+      <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>e26</t>
+        </is>
+      </c>
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr"/>
       <c r="O12" t="inlineStr">
         <is>
-          <t>End-to-end data-driven weather prediction</t>
+          <t>Reflective error: a metric for assessing predictive performance at extreme events</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
@@ -1073,12 +1085,12 @@
           <t>article</t>
         </is>
       </c>
-      <c r="Q12" t="inlineStr">
-        <is>
-          <t>https://www.nature.com/articles/s41586-025-08897-0</t>
-        </is>
-      </c>
-      <c r="R12" t="inlineStr"/>
+      <c r="Q12" t="inlineStr"/>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
       <c r="S12" t="inlineStr">
         <is>
           <t>2025</t>
@@ -1089,23 +1101,27 @@
       <c r="A13" t="inlineStr"/>
       <c r="B13" t="inlineStr">
         <is>
-          <t>R. C. Williams, P. Thodoroff, R. J. Arthern, J. Byrne, J. S. Hosking, M. Kaiser, N. D. Lawrence, I. Kazlauskaite</t>
+          <t>A. Allen, S. Markou, W. Tebbutt, J. Requeima, W. P. Bruinsma, T. R. Andersson, N. D. Herzog, M. Chantry, J. S. Hosking, R. E. Turner</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>10.1038/s43247-025-02010-z</t>
+          <t>https://doi.org/10.1038/s41586-025-08897-0</t>
         </is>
       </c>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Commun Earth Environ</t>
+          <t>Nature</t>
         </is>
       </c>
       <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Guardian, blue, https://www.theguardian.com/technology/2025/mar/20/ai-aardvark-weather-prediction-forecasting-artificial-intelligence; FT, DarkOrange, https://www.ft.com/content/73492128-5822-4bb2-b953-64217eb303e4; New Scientist, grey, https://www.newscientist.com/article/2472659-ai-can-forecast-the-weather-in-seconds-without-needing-supercomputers/; Independent, red, https://www.independent.co.uk/tech/ai-weather-forecast-aardvark-cambridge-b2717122.html; Blog, black, https://www.turing.ac.uk/blog/project-aardvark-reimagining-ai-weather-prediction</t>
+        </is>
+      </c>
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr"/>
@@ -1114,7 +1130,7 @@
       <c r="N13" t="inlineStr"/>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Calculations of extreme sea level rise scenarios are strongly dependent on ice sheet model resolution</t>
+          <t>End-to-end data-driven weather prediction</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
@@ -1124,7 +1140,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1038/s43247-025-02010-z</t>
+          <t>https://www.nature.com/articles/s41586-025-08897-0</t>
         </is>
       </c>
       <c r="R13" t="inlineStr"/>
@@ -1138,36 +1154,32 @@
       <c r="A14" t="inlineStr"/>
       <c r="B14" t="inlineStr">
         <is>
-          <t>R. E. Rouse, D. Khamis, S. Hosking, A. McRobie, E. Shuckburgh</t>
+          <t>R. C. Williams, P. Thodoroff, R. J. Arthern, J. Byrne, J. S. Hosking, M. Kaiser, N. D. Lawrence, I. Kazlauskaite</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>10.1017/eds.2024.48</t>
+          <t>10.1038/s43247-025-02010-z</t>
         </is>
       </c>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Environmental Data Science</t>
+          <t>Commun Earth Environ</t>
         </is>
       </c>
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr"/>
       <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr"/>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>e5</t>
-        </is>
-      </c>
+      <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr"/>
       <c r="M14" t="inlineStr"/>
       <c r="N14" t="inlineStr"/>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Streamflow prediction using artificial neural networks and soil moisture proxies</t>
+          <t>Calculations of extreme sea level rise scenarios are strongly dependent on ice sheet model resolution</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
@@ -1175,12 +1187,12 @@
           <t>article</t>
         </is>
       </c>
-      <c r="Q14" t="inlineStr"/>
-      <c r="R14" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1038/s43247-025-02010-z</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr"/>
       <c r="S14" t="inlineStr">
         <is>
           <t>2025</t>
@@ -1191,12 +1203,12 @@
       <c r="A15" t="inlineStr"/>
       <c r="B15" t="inlineStr">
         <is>
-          <t>A. Coca-Castro, A. Fouilloux, R. Barros Lourenço, A. McDonald, Y. Rao, J. S. Hosking</t>
+          <t>R. E. Rouse, D. Khamis, S. Hosking, A. McRobie, E. Shuckburgh</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>10.1017/eds.2024.35</t>
+          <t>10.1017/eds.2024.48</t>
         </is>
       </c>
       <c r="D15" t="inlineStr"/>
@@ -1210,13 +1222,17 @@
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr"/>
-      <c r="K15" t="inlineStr"/>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>e5</t>
+        </is>
+      </c>
       <c r="L15" t="inlineStr"/>
       <c r="M15" t="inlineStr"/>
       <c r="N15" t="inlineStr"/>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Improving the reproducibility in geoscientific papers: lessons learned from a Hackathon in climate science</t>
+          <t>Streamflow prediction using artificial neural networks and soil moisture proxies</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
@@ -1240,40 +1256,32 @@
       <c r="A16" t="inlineStr"/>
       <c r="B16" t="inlineStr">
         <is>
-          <t>K. Tazi, A. Orr, J. Hernandez-Gonz&amp;aacute;lez, S. Hosking, R. E. Turner</t>
+          <t>A. Coca-Castro, A. Fouilloux, R. Barros Lourenço, A. McDonald, Y. Rao, J. S. Hosking</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>10.5194/hess-28-4903-2024</t>
+          <t>10.1017/eds.2024.35</t>
         </is>
       </c>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Hydrology and Earth System Sciences</t>
+          <t>Environmental Data Science</t>
         </is>
       </c>
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>4903--4925</t>
-        </is>
-      </c>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr"/>
       <c r="M16" t="inlineStr"/>
       <c r="N16" t="inlineStr"/>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Downscaling precipitation over High-mountain Asia using multi-fidelity Gaussian processes: improved estimates from ERA5</t>
+          <t>Improving the reproducibility in geoscientific papers: lessons learned from a Hackathon in climate science</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
@@ -1281,19 +1289,15 @@
           <t>article</t>
         </is>
       </c>
-      <c r="Q16" t="inlineStr">
-        <is>
-          <t>https://hess.copernicus.org/articles/28/4903/2024/</t>
-        </is>
-      </c>
+      <c r="Q16" t="inlineStr"/>
       <c r="R16" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>4</t>
         </is>
       </c>
       <c r="S16" t="inlineStr">
         <is>
-          <t>2024</t>
+          <t>2025</t>
         </is>
       </c>
     </row>
@@ -1301,32 +1305,32 @@
       <c r="A17" t="inlineStr"/>
       <c r="B17" t="inlineStr">
         <is>
-          <t>M. S. Rogers, M. Fox, A. Fleming, L. {van Zeeland}, J. Wilkinson, J. S. Hosking</t>
+          <t>K. Tazi, A. Orr, J. Hernandez-Gonz&amp;aacute;lez, S. Hosking, R. E. Turner</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1016/j.rse.2024.114073</t>
+          <t>10.5194/hess-28-4903-2024</t>
         </is>
       </c>
       <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>0034-4257</t>
-        </is>
-      </c>
+      <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Remote Sensing of Environment</t>
+          <t>Hydrology and Earth System Sciences</t>
         </is>
       </c>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr"/>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>114073</t>
+          <t>4903--4925</t>
         </is>
       </c>
       <c r="L17" t="inlineStr"/>
@@ -1334,7 +1338,7 @@
       <c r="N17" t="inlineStr"/>
       <c r="O17" t="inlineStr">
         <is>
-          <t>Sea ice detection using concurrent multispectral and synthetic aperture radar imagery</t>
+          <t>Downscaling precipitation over High-mountain Asia using multi-fidelity Gaussian processes: improved estimates from ERA5</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
@@ -1344,12 +1348,12 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>https://www.sciencedirect.com/science/article/pii/S0034425724000841</t>
+          <t>https://hess.copernicus.org/articles/28/4903/2024/</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
         <is>
-          <t>305</t>
+          <t>28</t>
         </is>
       </c>
       <c r="S17" t="inlineStr">
@@ -1362,19 +1366,23 @@
       <c r="A18" t="inlineStr"/>
       <c r="B18" t="inlineStr">
         <is>
-          <t>H. L. Joakimsen, I. Martinsen, L. T. Luppino, A. McDonald, S. Hosking, R. Jenssen</t>
+          <t>M. S. Rogers, M. Fox, A. Fleming, L. {van Zeeland}, J. Wilkinson, J. S. Hosking</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>10.1109/LGRS.2024.3366308</t>
+          <t>https://doi.org/10.1016/j.rse.2024.114073</t>
         </is>
       </c>
       <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>0034-4257</t>
+        </is>
+      </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>IEEE Geoscience and Remote Sensing Letters</t>
+          <t>Remote Sensing of Environment</t>
         </is>
       </c>
       <c r="G18" t="inlineStr"/>
@@ -1383,7 +1391,7 @@
       <c r="J18" t="inlineStr"/>
       <c r="K18" t="inlineStr">
         <is>
-          <t>1-5</t>
+          <t>114073</t>
         </is>
       </c>
       <c r="L18" t="inlineStr"/>
@@ -1391,7 +1399,7 @@
       <c r="N18" t="inlineStr"/>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Interrogating Sea Ice Predictability With Gradients</t>
+          <t>Sea ice detection using concurrent multispectral and synthetic aperture radar imagery</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
@@ -1399,10 +1407,14 @@
           <t>article</t>
         </is>
       </c>
-      <c r="Q18" t="inlineStr"/>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>https://www.sciencedirect.com/science/article/pii/S0034425724000841</t>
+        </is>
+      </c>
       <c r="R18" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>305</t>
         </is>
       </c>
       <c r="S18" t="inlineStr">
@@ -1415,32 +1427,36 @@
       <c r="A19" t="inlineStr"/>
       <c r="B19" t="inlineStr">
         <is>
-          <t>C. Jay, Y. Yu, I. Crawford, S. Archer-Nicholls, P. James, A. Gledson, G. Shaddick, R. Haines, L. Lannelongue, E. Lines, S. Hosking, D. Topping</t>
+          <t>H. L. Joakimsen, I. Martinsen, L. T. Luppino, A. McDonald, S. Hosking, R. Jenssen</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>10.1038/s41561-023-01369-y</t>
+          <t>10.1109/LGRS.2024.3366308</t>
         </is>
       </c>
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Nature Geoscience</t>
+          <t>IEEE Geoscience and Remote Sensing Letters</t>
         </is>
       </c>
       <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr"/>
       <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr"/>
-      <c r="K19" t="inlineStr"/>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>1-5</t>
+        </is>
+      </c>
       <c r="L19" t="inlineStr"/>
       <c r="M19" t="inlineStr"/>
       <c r="N19" t="inlineStr"/>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Prioritize environmental sustainability in use of AI and data science methods</t>
+          <t>Interrogating Sea Ice Predictability With Gradients</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -1448,12 +1464,12 @@
           <t>article</t>
         </is>
       </c>
-      <c r="Q19" t="inlineStr">
-        <is>
-          <t>https://www.nature.com/articles/s41561-023-01369-y</t>
-        </is>
-      </c>
-      <c r="R19" t="inlineStr"/>
+      <c r="Q19" t="inlineStr"/>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
       <c r="S19" t="inlineStr">
         <is>
           <t>2024</t>
@@ -1464,44 +1480,32 @@
       <c r="A20" t="inlineStr"/>
       <c r="B20" t="inlineStr">
         <is>
-          <t>B. Evans, A. Faul, A. Fleming, D. G. Vaughan, J. S. Hosking</t>
+          <t>C. Jay, Y. Yu, I. Crawford, S. Archer-Nicholls, P. James, A. Gledson, G. Shaddick, R. Haines, L. Lannelongue, E. Lines, S. Hosking, D. Topping</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>10.1016/j.rse.2023.113780</t>
+          <t>10.1038/s41561-023-01369-y</t>
         </is>
       </c>
       <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>0034-4257</t>
-        </is>
-      </c>
+      <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Remote Sensing of Environment</t>
+          <t>Nature Geoscience</t>
         </is>
       </c>
       <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>Fox Weather, blue, https://www.foxweather.com/weather-news/iceberg-a23a-weddell-sea-antarctic-peninsula; Press Release, DarkOrange, https://www.bas.ac.uk/media-post/using-ai-to-track-icebergs/</t>
-        </is>
-      </c>
+      <c r="H20" t="inlineStr"/>
       <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr"/>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>113780</t>
-        </is>
-      </c>
+      <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr"/>
       <c r="M20" t="inlineStr"/>
       <c r="N20" t="inlineStr"/>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Unsupervised machine learning detection of iceberg populations within sea ice from dual-polarisation SAR imagery</t>
+          <t>Prioritize environmental sustainability in use of AI and data science methods</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
@@ -1511,17 +1515,13 @@
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>https://www.sciencedirect.com/science/article/pii/S0034425723003310</t>
-        </is>
-      </c>
-      <c r="R20" t="inlineStr">
-        <is>
-          <t>297</t>
-        </is>
-      </c>
+          <t>https://www.nature.com/articles/s41561-023-01369-y</t>
+        </is>
+      </c>
+      <c r="R20" t="inlineStr"/>
       <c r="S20" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>2024</t>
         </is>
       </c>
     </row>
@@ -1529,28 +1529,36 @@
       <c r="A21" t="inlineStr"/>
       <c r="B21" t="inlineStr">
         <is>
-          <t>T. R. Andersson, W. P. Bruinsma, S. Markou, J. Requeima, A. Coca-Castro, A. Vaughan, A.-L. Ellis, M. A. Lazzara, D. Jones, S. Hosking, R. E. Turner</t>
+          <t>B. Evans, A. Faul, A. Fleming, D. G. Vaughan, J. S. Hosking</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>10.1017/eds.2023.22</t>
+          <t>10.1016/j.rse.2023.113780</t>
         </is>
       </c>
       <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr"/>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>0034-4257</t>
+        </is>
+      </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Environmental Data Science</t>
+          <t>Remote Sensing of Environment</t>
         </is>
       </c>
       <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr"/>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Fox Weather, blue, https://www.foxweather.com/weather-news/iceberg-a23a-weddell-sea-antarctic-peninsula; Press Release, DarkOrange, https://www.bas.ac.uk/media-post/using-ai-to-track-icebergs/</t>
+        </is>
+      </c>
       <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr">
         <is>
-          <t>e32</t>
+          <t>113780</t>
         </is>
       </c>
       <c r="L21" t="inlineStr"/>
@@ -1558,7 +1566,7 @@
       <c r="N21" t="inlineStr"/>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Environmental sensor placement with convolutional Gaussian neural processes</t>
+          <t>Unsupervised machine learning detection of iceberg populations within sea ice from dual-polarisation SAR imagery</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -1566,10 +1574,14 @@
           <t>article</t>
         </is>
       </c>
-      <c r="Q21" t="inlineStr"/>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>https://www.sciencedirect.com/science/article/pii/S0034425723003310</t>
+        </is>
+      </c>
       <c r="R21" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>297</t>
         </is>
       </c>
       <c r="S21" t="inlineStr">
@@ -1582,32 +1594,28 @@
       <c r="A22" t="inlineStr"/>
       <c r="B22" t="inlineStr">
         <is>
-          <t>R. Parthipan, H. M. Christensen, J. S. Hosking, D. J. Wischik</t>
+          <t>T. R. Andersson, W. P. Bruinsma, S. Markou, J. Requeima, A. Coca-Castro, A. Vaughan, A.-L. Ellis, M. A. Lazzara, D. Jones, S. Hosking, R. E. Turner</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>10.5194/gmd-16-4501-2023</t>
+          <t>10.1017/eds.2023.22</t>
         </is>
       </c>
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Geoscientific Model Development</t>
+          <t>Environmental Data Science</t>
         </is>
       </c>
       <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr"/>
       <c r="I22" t="inlineStr"/>
-      <c r="J22" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
+      <c r="J22" t="inlineStr"/>
       <c r="K22" t="inlineStr">
         <is>
-          <t>4501--4519</t>
+          <t>e32</t>
         </is>
       </c>
       <c r="L22" t="inlineStr"/>
@@ -1615,7 +1623,7 @@
       <c r="N22" t="inlineStr"/>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Using probabilistic machine learning to better model temporal patterns in parameterizations: a case study with the Lorenz 96 model</t>
+          <t>Environmental sensor placement with convolutional Gaussian neural processes</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
@@ -1623,14 +1631,10 @@
           <t>article</t>
         </is>
       </c>
-      <c r="Q22" t="inlineStr">
-        <is>
-          <t>https://gmd.copernicus.org/articles/16/4501/2023/</t>
-        </is>
-      </c>
+      <c r="Q22" t="inlineStr"/>
       <c r="R22" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>2</t>
         </is>
       </c>
       <c r="S22" t="inlineStr">
@@ -1643,32 +1647,40 @@
       <c r="A23" t="inlineStr"/>
       <c r="B23" t="inlineStr">
         <is>
-          <t>W. P. Bruinsma, S. Markou, J. Requiema, A. Y. Foong, T. R. Andersson, A. Vaughan, A. Buonomo, J. S. Hosking, R. E. Turner</t>
+          <t>R. Parthipan, H. M. Christensen, J. S. Hosking, D. J. Wischik</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>10.48550/arXiv.2303.14468</t>
+          <t>10.5194/gmd-16-4501-2023</t>
         </is>
       </c>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr">
         <is>
-          <t>11th International Conference on Learning Representations (ICLR 2023)</t>
+          <t>Geoscientific Model Development</t>
         </is>
       </c>
       <c r="G23" t="inlineStr"/>
       <c r="H23" t="inlineStr"/>
       <c r="I23" t="inlineStr"/>
-      <c r="J23" t="inlineStr"/>
-      <c r="K23" t="inlineStr"/>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>4501--4519</t>
+        </is>
+      </c>
       <c r="L23" t="inlineStr"/>
       <c r="M23" t="inlineStr"/>
       <c r="N23" t="inlineStr"/>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Autoregressive Conditional Neural Processes</t>
+          <t>Using probabilistic machine learning to better model temporal patterns in parameterizations: a case study with the Lorenz 96 model</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -1676,8 +1688,16 @@
           <t>article</t>
         </is>
       </c>
-      <c r="Q23" t="inlineStr"/>
-      <c r="R23" t="inlineStr"/>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>https://gmd.copernicus.org/articles/16/4501/2023/</t>
+        </is>
+      </c>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
       <c r="S23" t="inlineStr">
         <is>
           <t>2023</t>
@@ -1688,40 +1708,32 @@
       <c r="A24" t="inlineStr"/>
       <c r="B24" t="inlineStr">
         <is>
-          <t>T. Summers, E. Mackie, R. Ueno, C. Simpson, J. S. Hosking, T. Suciu, A. Coburn, E. Shuckburgh</t>
+          <t>W. P. Bruinsma, S. Markou, J. Requiema, A. Y. Foong, T. R. Andersson, A. Vaughan, A. Buonomo, J. S. Hosking, R. E. Turner</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>10.1002/cli2.35</t>
+          <t>10.48550/arXiv.2303.14468</t>
         </is>
       </c>
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Climate Resilience and Sustainability</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>bias, climate, correction, disruption, economic, exceedance, temperature</t>
-        </is>
-      </c>
+          <t>11th International Conference on Learning Representations (ICLR 2023)</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr"/>
       <c r="J24" t="inlineStr"/>
-      <c r="K24" t="inlineStr">
-        <is>
-          <t>e35</t>
-        </is>
-      </c>
+      <c r="K24" t="inlineStr"/>
       <c r="L24" t="inlineStr"/>
       <c r="M24" t="inlineStr"/>
       <c r="N24" t="inlineStr"/>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Localized impacts and economic implications from high temperature disruption days under climate change</t>
+          <t>Autoregressive Conditional Neural Processes</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
@@ -1729,15 +1741,11 @@
           <t>article</t>
         </is>
       </c>
-      <c r="Q24" t="inlineStr">
-        <is>
-          <t>https://rmets.onlinelibrary.wiley.com/doi/abs/10.1002/cli2.35</t>
-        </is>
-      </c>
+      <c r="Q24" t="inlineStr"/>
       <c r="R24" t="inlineStr"/>
       <c r="S24" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2023</t>
         </is>
       </c>
     </row>
@@ -1745,32 +1753,32 @@
       <c r="A25" t="inlineStr"/>
       <c r="B25" t="inlineStr">
         <is>
-          <t>A. Vaughan, W. Tebbutt, J. S. Hosking, R. E. Turner</t>
+          <t>T. Summers, E. Mackie, R. Ueno, C. Simpson, J. S. Hosking, T. Suciu, A. Coburn, E. Shuckburgh</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>10.5194/gmd-15-251-2022</t>
+          <t>10.1002/cli2.35</t>
         </is>
       </c>
       <c r="D25" t="inlineStr"/>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Geoscientific Model Development</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr"/>
+          <t>Climate Resilience and Sustainability</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>bias, climate, correction, disruption, economic, exceedance, temperature</t>
+        </is>
+      </c>
       <c r="H25" t="inlineStr"/>
       <c r="I25" t="inlineStr"/>
-      <c r="J25" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
+      <c r="J25" t="inlineStr"/>
       <c r="K25" t="inlineStr">
         <is>
-          <t>251--268</t>
+          <t>e35</t>
         </is>
       </c>
       <c r="L25" t="inlineStr"/>
@@ -1778,7 +1786,7 @@
       <c r="N25" t="inlineStr"/>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Convolutional conditional neural processes for local climate downscaling</t>
+          <t>Localized impacts and economic implications from high temperature disruption days under climate change</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
@@ -1788,14 +1796,10 @@
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>https://gmd.copernicus.org/articles/15/251/2022/</t>
-        </is>
-      </c>
-      <c r="R25" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
+          <t>https://rmets.onlinelibrary.wiley.com/doi/abs/10.1002/cli2.35</t>
+        </is>
+      </c>
+      <c r="R25" t="inlineStr"/>
       <c r="S25" t="inlineStr">
         <is>
           <t>2022</t>
@@ -1806,36 +1810,32 @@
       <c r="A26" t="inlineStr"/>
       <c r="B26" t="inlineStr">
         <is>
-          <t>C. Simpson, J. S. Hosking, D. Mitchell, R. A. Betts, E. Shuckburgh</t>
+          <t>A. Vaughan, W. Tebbutt, J. S. Hosking, R. E. Turner</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>10.1088/1748-9326/ac3288</t>
+          <t>10.5194/gmd-15-251-2022</t>
         </is>
       </c>
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Environmental Research Letters</t>
+          <t>Geoscientific Model Development</t>
         </is>
       </c>
       <c r="G26" t="inlineStr"/>
       <c r="H26" t="inlineStr"/>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>nov</t>
-        </is>
-      </c>
+      <c r="I26" t="inlineStr"/>
       <c r="J26" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>124004</t>
+          <t>251--268</t>
         </is>
       </c>
       <c r="L26" t="inlineStr"/>
@@ -1843,7 +1843,7 @@
       <c r="N26" t="inlineStr"/>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Regional disparities and seasonal differences in climate risk to rice labour</t>
+          <t>Convolutional conditional neural processes for local climate downscaling</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
@@ -1853,17 +1853,17 @@
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1088/1748-9326/ac3288</t>
+          <t>https://gmd.copernicus.org/articles/15/251/2022/</t>
         </is>
       </c>
       <c r="R26" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>15</t>
         </is>
       </c>
       <c r="S26" t="inlineStr">
         <is>
-          <t>2021</t>
+          <t>2022</t>
         </is>
       </c>
     </row>
@@ -1871,40 +1871,44 @@
       <c r="A27" t="inlineStr"/>
       <c r="B27" t="inlineStr">
         <is>
-          <t>N. Eastwood, W. A. Stubbings, M. A. {Abou-Elwafa Abdallah}, I. Durance, J. Paavola, M. Dallimer, J. H. Pantel, S. Johnson, J. Zhou, J. S. Hosking, J. B. Brown, S. Ullah, S. Krause, D. M. Hannah, S. E. Crawford, M. Widmann, L. Orsini</t>
+          <t>C. Simpson, J. S. Hosking, D. Mitchell, R. A. Betts, E. Shuckburgh</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1016/j.tree.2021.09.008</t>
+          <t>10.1088/1748-9326/ac3288</t>
         </is>
       </c>
       <c r="D27" t="inlineStr"/>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>0169-5347</t>
-        </is>
-      </c>
+      <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Trends in Ecology &amp; Evolution</t>
+          <t>Environmental Research Letters</t>
         </is>
       </c>
       <c r="G27" t="inlineStr"/>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>The New Stack, HotPink, https://thenewstack.io/ai-biodiversity-time-machine-could-decide-for-uncertain-future/</t>
-        </is>
-      </c>
-      <c r="I27" t="inlineStr"/>
-      <c r="J27" t="inlineStr"/>
-      <c r="K27" t="inlineStr"/>
+      <c r="H27" t="inlineStr"/>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>nov</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>124004</t>
+        </is>
+      </c>
       <c r="L27" t="inlineStr"/>
       <c r="M27" t="inlineStr"/>
       <c r="N27" t="inlineStr"/>
       <c r="O27" t="inlineStr">
         <is>
-          <t>The Time Machine framework: monitoring and prediction of biodiversity loss</t>
+          <t>Regional disparities and seasonal differences in climate risk to rice labour</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
@@ -1914,10 +1918,14 @@
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>https://www.sciencedirect.com/science/article/pii/S0169534721002597</t>
-        </is>
-      </c>
-      <c r="R27" t="inlineStr"/>
+          <t>https://doi.org/10.1088/1748-9326/ac3288</t>
+        </is>
+      </c>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
       <c r="S27" t="inlineStr">
         <is>
           <t>2021</t>
@@ -1928,25 +1936,29 @@
       <c r="A28" t="inlineStr"/>
       <c r="B28" t="inlineStr">
         <is>
-          <t>T. Andersson, J. S. Hosking, M. Pérez-Ortiz, B. Paige, A. Elliott, C. Russell, S. Law, D. C. Jones, J. Wilkinson, T. Phillips, J. Byrne, S. Tietsche, B. B. Sarojini, E. Blanchard-Wrigglesworth, Y. Aksenov, R. Downie, E. Shuckburgh</t>
+          <t>N. Eastwood, W. A. Stubbings, M. A. {Abou-Elwafa Abdallah}, I. Durance, J. Paavola, M. Dallimer, J. H. Pantel, S. Johnson, J. Zhou, J. S. Hosking, J. B. Brown, S. Ullah, S. Krause, D. M. Hannah, S. E. Crawford, M. Widmann, L. Orsini</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1038/s41467-021-25257-4</t>
+          <t>https://doi.org/10.1016/j.tree.2021.09.008</t>
         </is>
       </c>
       <c r="D28" t="inlineStr"/>
-      <c r="E28" t="inlineStr"/>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>0169-5347</t>
+        </is>
+      </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Nature Communications</t>
+          <t>Trends in Ecology &amp; Evolution</t>
         </is>
       </c>
       <c r="G28" t="inlineStr"/>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Nvidia Blog, green, https://blogs.nvidia.com/blog/2021/08/31/ai-model-predicts-sea-ice-loss/; Wired, black, https://www.wired.com/story/as-the-arctic-warms-ai-forecasts-scope-out-shifting-sea-ice/; Science News, blue, https://www.sciencenews.org/article/artificial-intelligence-sea-ice-forecast; Eos, grey, https://eos.org/articles/could-ai-be-useful-for-arctic-communities-facing-sea-ice-loss; BBC Podcast, red, https://www.bbc.co.uk/programmes/w3ct1lsl; Mail Online, DarkOrange, https://www.dailymail.co.uk/sciencetech/article-9928807/British-Antarctic-Survey-builds-AI-predict-ice-loss.html</t>
+          <t>The New Stack, HotPink, https://thenewstack.io/ai-biodiversity-time-machine-could-decide-for-uncertain-future/</t>
         </is>
       </c>
       <c r="I28" t="inlineStr"/>
@@ -1957,7 +1969,7 @@
       <c r="N28" t="inlineStr"/>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Seasonal Arctic sea ice forecasting with probabilistic deep learning</t>
+          <t>The Time Machine framework: monitoring and prediction of biodiversity loss</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
@@ -1967,7 +1979,7 @@
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>https://www.nature.com/articles/s41467-021-25257-4</t>
+          <t>https://www.sciencedirect.com/science/article/pii/S0169534721002597</t>
         </is>
       </c>
       <c r="R28" t="inlineStr"/>
@@ -1981,40 +1993,36 @@
       <c r="A29" t="inlineStr"/>
       <c r="B29" t="inlineStr">
         <is>
-          <t>J. C. King, J. Turner, S. Colwell, H. Lu, A. Orr, T. Phillips, J. S. Hosking, G. J. Marshall</t>
+          <t>T. Andersson, J. S. Hosking, M. Pérez-Ortiz, B. Paige, A. Elliott, C. Russell, S. Law, D. C. Jones, J. Wilkinson, T. Phillips, J. Byrne, S. Tietsche, B. B. Sarojini, E. Blanchard-Wrigglesworth, Y. Aksenov, R. Downie, E. Shuckburgh</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>10.1175/JCLI-D-20-0748.1</t>
+          <t>https://doi.org/10.1038/s41467-021-25257-4</t>
         </is>
       </c>
       <c r="D29" t="inlineStr"/>
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Journal of Climate</t>
+          <t>Nature Communications</t>
         </is>
       </c>
       <c r="G29" t="inlineStr"/>
-      <c r="H29" t="inlineStr"/>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Nvidia Blog, green, https://blogs.nvidia.com/blog/2021/08/31/ai-model-predicts-sea-ice-loss/; Wired, black, https://www.wired.com/story/as-the-arctic-warms-ai-forecasts-scope-out-shifting-sea-ice/; Science News, blue, https://www.sciencenews.org/article/artificial-intelligence-sea-ice-forecast; Eos, grey, https://eos.org/articles/could-ai-be-useful-for-arctic-communities-facing-sea-ice-loss; BBC Podcast, red, https://www.bbc.co.uk/programmes/w3ct1lsl; Mail Online, DarkOrange, https://www.dailymail.co.uk/sciencetech/article-9928807/British-Antarctic-Survey-builds-AI-predict-ice-loss.html</t>
+        </is>
+      </c>
       <c r="I29" t="inlineStr"/>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="K29" t="inlineStr">
-        <is>
-          <t>4771 - 4783</t>
-        </is>
-      </c>
+      <c r="J29" t="inlineStr"/>
+      <c r="K29" t="inlineStr"/>
       <c r="L29" t="inlineStr"/>
       <c r="M29" t="inlineStr"/>
       <c r="N29" t="inlineStr"/>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Inhomogeneity of the Surface Air Temperature Record from Halley, Antarctica</t>
+          <t>Seasonal Arctic sea ice forecasting with probabilistic deep learning</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
@@ -2024,14 +2032,10 @@
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>https://journals.ametsoc.org/view/journals/clim/34/12/JCLI-D-20-0748.1.xml</t>
-        </is>
-      </c>
-      <c r="R29" t="inlineStr">
-        <is>
-          <t>34</t>
-        </is>
-      </c>
+          <t>https://www.nature.com/articles/s41467-021-25257-4</t>
+        </is>
+      </c>
+      <c r="R29" t="inlineStr"/>
       <c r="S29" t="inlineStr">
         <is>
           <t>2021</t>
@@ -2042,19 +2046,19 @@
       <c r="A30" t="inlineStr"/>
       <c r="B30" t="inlineStr">
         <is>
-          <t>S. E. Haupt, W. Chapman, S. V. Adams, C. Kirkwood, J. S. Hosking, N. H. Robinson, S. Lerch, A. C. Subramanian</t>
+          <t>J. C. King, J. Turner, S. Colwell, H. Lu, A. Orr, T. Phillips, J. S. Hosking, G. J. Marshall</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>10.1098/rsta.2020.0091</t>
+          <t>10.1175/JCLI-D-20-0748.1</t>
         </is>
       </c>
       <c r="D30" t="inlineStr"/>
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Philosophical Transactions of the Royal Society A: Mathematical, Physical and Engineering Sciences</t>
+          <t>Journal of Climate</t>
         </is>
       </c>
       <c r="G30" t="inlineStr"/>
@@ -2062,12 +2066,12 @@
       <c r="I30" t="inlineStr"/>
       <c r="J30" t="inlineStr">
         <is>
-          <t>2194</t>
+          <t>12</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>20200091</t>
+          <t>4771 - 4783</t>
         </is>
       </c>
       <c r="L30" t="inlineStr"/>
@@ -2075,7 +2079,7 @@
       <c r="N30" t="inlineStr"/>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Towards implementing artificial intelligence post-processing in weather and climate: proposed actions from the Oxford 2019 workshop</t>
+          <t>Inhomogeneity of the Surface Air Temperature Record from Halley, Antarctica</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
@@ -2085,12 +2089,12 @@
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>https://royalsocietypublishing.org/doi/abs/10.1098/rsta.2020.0091</t>
+          <t>https://journals.ametsoc.org/view/journals/clim/34/12/JCLI-D-20-0748.1.xml</t>
         </is>
       </c>
       <c r="R30" t="inlineStr">
         <is>
-          <t>379</t>
+          <t>34</t>
         </is>
       </c>
       <c r="S30" t="inlineStr">
@@ -2103,28 +2107,40 @@
       <c r="A31" t="inlineStr"/>
       <c r="B31" t="inlineStr">
         <is>
-          <t>U. Sengupta, M. Amos, J. S. Hosking, C. E. Rasmussen, M. Juniper, P. J. Young</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr"/>
+          <t>S. E. Haupt, W. Chapman, S. V. Adams, C. Kirkwood, J. S. Hosking, N. H. Robinson, S. Lerch, A. C. Subramanian</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>10.1098/rsta.2020.0091</t>
+        </is>
+      </c>
       <c r="D31" t="inlineStr"/>
       <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Advances in Neural Information Processing Systems (NeurIPS) 2020</t>
+          <t>Philosophical Transactions of the Royal Society A: Mathematical, Physical and Engineering Sciences</t>
         </is>
       </c>
       <c r="G31" t="inlineStr"/>
       <c r="H31" t="inlineStr"/>
       <c r="I31" t="inlineStr"/>
-      <c r="J31" t="inlineStr"/>
-      <c r="K31" t="inlineStr"/>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>2194</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>20200091</t>
+        </is>
+      </c>
       <c r="L31" t="inlineStr"/>
       <c r="M31" t="inlineStr"/>
       <c r="N31" t="inlineStr"/>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Ensembling geophysical models with Bayesian Neural Networks</t>
+          <t>Towards implementing artificial intelligence post-processing in weather and climate: proposed actions from the Oxford 2019 workshop</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
@@ -2134,13 +2150,17 @@
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>https://arxiv.org/abs/2010.03561v1</t>
-        </is>
-      </c>
-      <c r="R31" t="inlineStr"/>
+          <t>https://royalsocietypublishing.org/doi/abs/10.1098/rsta.2020.0091</t>
+        </is>
+      </c>
+      <c r="R31" t="inlineStr">
+        <is>
+          <t>379</t>
+        </is>
+      </c>
       <c r="S31" t="inlineStr">
         <is>
-          <t>2020</t>
+          <t>2021</t>
         </is>
       </c>
     </row>
@@ -2148,7 +2168,7 @@
       <c r="A32" t="inlineStr"/>
       <c r="B32" t="inlineStr">
         <is>
-          <t>W. P. Bruinsma, E. Perim, W. Tebbutt, J. S. Hosking, A. Solin, R. E. Turner</t>
+          <t>U. Sengupta, M. Amos, J. S. Hosking, C. E. Rasmussen, M. Juniper, P. J. Young</t>
         </is>
       </c>
       <c r="C32" t="inlineStr"/>
@@ -2156,7 +2176,7 @@
       <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Proceedings of the 37th International Conference on Machine Learning, Vienna, Austria, PMLR 119, 2020</t>
+          <t>Advances in Neural Information Processing Systems (NeurIPS) 2020</t>
         </is>
       </c>
       <c r="G32" t="inlineStr"/>
@@ -2169,7 +2189,7 @@
       <c r="N32" t="inlineStr"/>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Scalable Exact Inference in Multi-Output Gaussian Processes</t>
+          <t>Ensembling geophysical models with Bayesian Neural Networks</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
@@ -2179,7 +2199,7 @@
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>https://arxiv.org/abs/1911.06287</t>
+          <t>https://arxiv.org/abs/2010.03561v1</t>
         </is>
       </c>
       <c r="R32" t="inlineStr"/>
@@ -2193,40 +2213,28 @@
       <c r="A33" t="inlineStr"/>
       <c r="B33" t="inlineStr">
         <is>
-          <t>A. Orr, J. S. Hosking, A. Delon, L. Hoffmann, R. Spang, T. Moffat-Griffin, J. Keeble, N. L. Abraham, P. Braesicke</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>10.5194/acp-20-12483-2020</t>
-        </is>
-      </c>
+          <t>W. P. Bruinsma, E. Perim, W. Tebbutt, J. S. Hosking, A. Solin, R. E. Turner</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr"/>
       <c r="D33" t="inlineStr"/>
       <c r="E33" t="inlineStr"/>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Atmospheric Chemistry and Physics</t>
+          <t>Proceedings of the 37th International Conference on Machine Learning, Vienna, Austria, PMLR 119, 2020</t>
         </is>
       </c>
       <c r="G33" t="inlineStr"/>
       <c r="H33" t="inlineStr"/>
       <c r="I33" t="inlineStr"/>
-      <c r="J33" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
-      </c>
-      <c r="K33" t="inlineStr">
-        <is>
-          <t>12483--12497</t>
-        </is>
-      </c>
+      <c r="J33" t="inlineStr"/>
+      <c r="K33" t="inlineStr"/>
       <c r="L33" t="inlineStr"/>
       <c r="M33" t="inlineStr"/>
       <c r="N33" t="inlineStr"/>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Polar stratospheric clouds initiated by mountain waves in a global chemistry--climate model: a missing piece in fully modelling polar stratospheric ozone depletion</t>
+          <t>Scalable Exact Inference in Multi-Output Gaussian Processes</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
@@ -2236,14 +2244,10 @@
       </c>
       <c r="Q33" t="inlineStr">
         <is>
-          <t>https://acp.copernicus.org/articles/20/12483/2020/</t>
-        </is>
-      </c>
-      <c r="R33" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
+          <t>https://arxiv.org/abs/1911.06287</t>
+        </is>
+      </c>
+      <c r="R33" t="inlineStr"/>
       <c r="S33" t="inlineStr">
         <is>
           <t>2020</t>
@@ -2254,12 +2258,12 @@
       <c r="A34" t="inlineStr"/>
       <c r="B34" t="inlineStr">
         <is>
-          <t>M. Amos, P. J. Young, J. S. Hosking, J.-F. Lamarque, N. L. Abraham, H. Akiyoshi, A. T. Archibald, S. Bekki, M. Deushi, P. J&amp;ouml;ckel, D. Kinnison, O. Kirner, M. Kunze, M. Marchand, D. A. Plummer, D. Saint-Martin, K. Sudo, S. Tilmes, Y. Yamashita</t>
+          <t>A. Orr, J. S. Hosking, A. Delon, L. Hoffmann, R. Spang, T. Moffat-Griffin, J. Keeble, N. L. Abraham, P. Braesicke</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>10.5194/acp-20-9961-2020</t>
+          <t>10.5194/acp-20-12483-2020</t>
         </is>
       </c>
       <c r="D34" t="inlineStr"/>
@@ -2274,12 +2278,12 @@
       <c r="I34" t="inlineStr"/>
       <c r="J34" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>21</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>9961--9977</t>
+          <t>12483--12497</t>
         </is>
       </c>
       <c r="L34" t="inlineStr"/>
@@ -2287,7 +2291,7 @@
       <c r="N34" t="inlineStr"/>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Projecting ozone hole recovery using an ensemble of chemistry-climate models weighted by model performance and independence</t>
+          <t>Polar stratospheric clouds initiated by mountain waves in a global chemistry--climate model: a missing piece in fully modelling polar stratospheric ozone depletion</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
@@ -2297,7 +2301,7 @@
       </c>
       <c r="Q34" t="inlineStr">
         <is>
-          <t>https://acp.copernicus.org/articles/20/9961/2020/</t>
+          <t>https://acp.copernicus.org/articles/20/12483/2020/</t>
         </is>
       </c>
       <c r="R34" t="inlineStr">
@@ -2315,19 +2319,19 @@
       <c r="A35" t="inlineStr"/>
       <c r="B35" t="inlineStr">
         <is>
-          <t>T. J. Bracegirdle, C. R. Holmes, J. S. Hosking, G. J. Marshall, M. Osman, M. Patterson, T. Rackow</t>
+          <t>M. Amos, P. J. Young, J. S. Hosking, J.-F. Lamarque, N. L. Abraham, H. Akiyoshi, A. T. Archibald, S. Bekki, M. Deushi, P. J&amp;ouml;ckel, D. Kinnison, O. Kirner, M. Kunze, M. Marchand, D. A. Plummer, D. Saint-Martin, K. Sudo, S. Tilmes, Y. Yamashita</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>10.1029/2019EA001065</t>
+          <t>10.5194/acp-20-9961-2020</t>
         </is>
       </c>
       <c r="D35" t="inlineStr"/>
       <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Earth and Space Science</t>
+          <t>Atmospheric Chemistry and Physics</t>
         </is>
       </c>
       <c r="G35" t="inlineStr"/>
@@ -2335,12 +2339,12 @@
       <c r="I35" t="inlineStr"/>
       <c r="J35" t="inlineStr">
         <is>
-          <t>n/a</t>
+          <t>16</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>e2019EA001065</t>
+          <t>9961--9977</t>
         </is>
       </c>
       <c r="L35" t="inlineStr"/>
@@ -2348,7 +2352,7 @@
       <c r="N35" t="inlineStr"/>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Improvements in Circumpolar Southern Hemisphere Extratropical Atmospheric Circulation in CMIP6 Compared to CMIP5</t>
+          <t>Projecting ozone hole recovery using an ensemble of chemistry-climate models weighted by model performance and independence</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
@@ -2358,12 +2362,12 @@
       </c>
       <c r="Q35" t="inlineStr">
         <is>
-          <t>https://agupubs.onlinelibrary.wiley.com/doi/abs/10.1029/2019EA001065</t>
+          <t>https://acp.copernicus.org/articles/20/9961/2020/</t>
         </is>
       </c>
       <c r="R35" t="inlineStr">
         <is>
-          <t>n/a</t>
+          <t>20</t>
         </is>
       </c>
       <c r="S35" t="inlineStr">
@@ -2376,19 +2380,19 @@
       <c r="A36" t="inlineStr"/>
       <c r="B36" t="inlineStr">
         <is>
-          <t>M. R. McCrystall, J. S. Hosking, I. P. White, A. C. Maycock</t>
+          <t>T. J. Bracegirdle, C. R. Holmes, J. S. Hosking, G. J. Marshall, M. Osman, M. Patterson, T. Rackow</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>10.1175/JCLI-D-19-0456.1</t>
+          <t>10.1029/2019EA001065</t>
         </is>
       </c>
       <c r="D36" t="inlineStr"/>
       <c r="E36" t="inlineStr"/>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Journal of Climate</t>
+          <t>Earth and Space Science</t>
         </is>
       </c>
       <c r="G36" t="inlineStr"/>
@@ -2396,12 +2400,12 @@
       <c r="I36" t="inlineStr"/>
       <c r="J36" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>n/a</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>null</t>
+          <t>e2019EA001065</t>
         </is>
       </c>
       <c r="L36" t="inlineStr"/>
@@ -2409,7 +2413,7 @@
       <c r="N36" t="inlineStr"/>
       <c r="O36" t="inlineStr">
         <is>
-          <t>The impact of changes in tropical sea surface temperatures over 1979-2012 on Northern hemisphere high latitude climate</t>
+          <t>Improvements in Circumpolar Southern Hemisphere Extratropical Atmospheric Circulation in CMIP6 Compared to CMIP5</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
@@ -2419,12 +2423,12 @@
       </c>
       <c r="Q36" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1175/JCLI-D-19-0456.1</t>
+          <t>https://agupubs.onlinelibrary.wiley.com/doi/abs/10.1029/2019EA001065</t>
         </is>
       </c>
       <c r="R36" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>n/a</t>
         </is>
       </c>
       <c r="S36" t="inlineStr">
@@ -2437,28 +2441,40 @@
       <c r="A37" t="inlineStr"/>
       <c r="B37" t="inlineStr">
         <is>
-          <t>L. Kapetas, N. Kazakis, K. Voudouris, A. T. Martinez, J. S. Hosking</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr"/>
+          <t>M. R. McCrystall, J. S. Hosking, I. P. White, A. C. Maycock</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>10.1175/JCLI-D-19-0456.1</t>
+        </is>
+      </c>
       <c r="D37" t="inlineStr"/>
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr">
         <is>
-          <t>ICONHIC 2019: 2nd International Conference on Natural Hazards &amp; Infrastructure, Chania, Greece</t>
+          <t>Journal of Climate</t>
         </is>
       </c>
       <c r="G37" t="inlineStr"/>
       <c r="H37" t="inlineStr"/>
       <c r="I37" t="inlineStr"/>
-      <c r="J37" t="inlineStr"/>
-      <c r="K37" t="inlineStr"/>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
       <c r="L37" t="inlineStr"/>
       <c r="M37" t="inlineStr"/>
       <c r="N37" t="inlineStr"/>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Modelling Groundwater - Surface Water Interactions Under Climate Change Scenarios: insights from Axios Delta, Greece</t>
+          <t>The impact of changes in tropical sea surface temperatures over 1979-2012 on Northern hemisphere high latitude climate</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
@@ -2468,13 +2484,17 @@
       </c>
       <c r="Q37" t="inlineStr">
         <is>
-          <t>https://www.researchgate.net/profile/K_Voudouris/publication/334130545_Modelling_Groundwater_-Surface_Water_Interactions_Under_Climate_Change_Scenarios_insights_from_Axios_Delta_Greece/links/5d19a640458515c11c06bd23/Modelling-Groundwater-Surface-Water-Interactions-Under-Climate-Change-Scenarios-insights-from-Axios-Delta-Greece.pdf</t>
-        </is>
-      </c>
-      <c r="R37" t="inlineStr"/>
+          <t>https://doi.org/10.1175/JCLI-D-19-0456.1</t>
+        </is>
+      </c>
+      <c r="R37" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
       <c r="S37" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>2020</t>
         </is>
       </c>
     </row>
@@ -2482,36 +2502,28 @@
       <c r="A38" t="inlineStr"/>
       <c r="B38" t="inlineStr">
         <is>
-          <t>D. Bannister, A. Orr, S. K. Jain, I. P. Holman, A. Momblanch, T. Phillips, A. J. Adeloye, B. Snapir, T. W. Waine, J. S. Hosking, C. Allen-Sader</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>10.1029/2019JD030804</t>
-        </is>
-      </c>
+          <t>L. Kapetas, N. Kazakis, K. Voudouris, A. T. Martinez, J. S. Hosking</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr"/>
       <c r="D38" t="inlineStr"/>
       <c r="E38" t="inlineStr"/>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Journal of Geophysical Research: Atmospheres</t>
+          <t>ICONHIC 2019: 2nd International Conference on Natural Hazards &amp; Infrastructure, Chania, Greece</t>
         </is>
       </c>
       <c r="G38" t="inlineStr"/>
       <c r="H38" t="inlineStr"/>
       <c r="I38" t="inlineStr"/>
-      <c r="J38" t="inlineStr">
-        <is>
-          <t>n/a</t>
-        </is>
-      </c>
+      <c r="J38" t="inlineStr"/>
       <c r="K38" t="inlineStr"/>
       <c r="L38" t="inlineStr"/>
       <c r="M38" t="inlineStr"/>
       <c r="N38" t="inlineStr"/>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Bias correction of high-resolution regional climate model precipitation output gives the best estimates of precipitation in Himalayan catchments</t>
+          <t>Modelling Groundwater - Surface Water Interactions Under Climate Change Scenarios: insights from Axios Delta, Greece</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
@@ -2521,14 +2533,10 @@
       </c>
       <c r="Q38" t="inlineStr">
         <is>
-          <t>https://agupubs.onlinelibrary.wiley.com/doi/abs/10.1029/2019JD030804</t>
-        </is>
-      </c>
-      <c r="R38" t="inlineStr">
-        <is>
-          <t>n/a</t>
-        </is>
-      </c>
+          <t>https://www.researchgate.net/profile/K_Voudouris/publication/334130545_Modelling_Groundwater_-Surface_Water_Interactions_Under_Climate_Change_Scenarios_insights_from_Axios_Delta_Greece/links/5d19a640458515c11c06bd23/Modelling-Groundwater-Surface-Water-Interactions-Under-Climate-Change-Scenarios-insights-from-Axios-Delta-Greece.pdf</t>
+        </is>
+      </c>
+      <c r="R38" t="inlineStr"/>
       <c r="S38" t="inlineStr">
         <is>
           <t>2019</t>
@@ -2539,44 +2547,36 @@
       <c r="A39" t="inlineStr"/>
       <c r="B39" t="inlineStr">
         <is>
-          <t>J. Turner, T. Phillips, M. Thamban, W. Rahaman, G. J. Marshall, J. D. Wille, V. Favier, V. H. Winton, E. Thomas, Z. Wang, M. Broeke, J. S. Hosking, T. Lachlan-Cope</t>
+          <t>D. Bannister, A. Orr, S. K. Jain, I. P. Holman, A. Momblanch, T. Phillips, A. J. Adeloye, B. Snapir, T. W. Waine, J. S. Hosking, C. Allen-Sader</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>10.1029/2018GL081517</t>
+          <t>10.1029/2019JD030804</t>
         </is>
       </c>
       <c r="D39" t="inlineStr"/>
       <c r="E39" t="inlineStr"/>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Geophysical Research Letters</t>
+          <t>Journal of Geophysical Research: Atmospheres</t>
         </is>
       </c>
       <c r="G39" t="inlineStr"/>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>Phys.org, black, https://phys.org/news/2019-03-antarctic-snowfall-dominated-extreme-snowstorms.html</t>
-        </is>
-      </c>
+      <c r="H39" t="inlineStr"/>
       <c r="I39" t="inlineStr"/>
       <c r="J39" t="inlineStr">
         <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="K39" t="inlineStr">
-        <is>
-          <t>3502-3511</t>
-        </is>
-      </c>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr"/>
       <c r="L39" t="inlineStr"/>
       <c r="M39" t="inlineStr"/>
       <c r="N39" t="inlineStr"/>
       <c r="O39" t="inlineStr">
         <is>
-          <t>The Dominant Role of Extreme Precipitation Events in Antarctic Snowfall Variability</t>
+          <t>Bias correction of high-resolution regional climate model precipitation output gives the best estimates of precipitation in Himalayan catchments</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
@@ -2586,12 +2586,12 @@
       </c>
       <c r="Q39" t="inlineStr">
         <is>
-          <t>https://agupubs.onlinelibrary.wiley.com/doi/abs/10.1029/2018GL081517</t>
+          <t>https://agupubs.onlinelibrary.wiley.com/doi/abs/10.1029/2019JD030804</t>
         </is>
       </c>
       <c r="R39" t="inlineStr">
         <is>
-          <t>46</t>
+          <t>n/a</t>
         </is>
       </c>
       <c r="S39" t="inlineStr">
@@ -2604,12 +2604,12 @@
       <c r="A40" t="inlineStr"/>
       <c r="B40" t="inlineStr">
         <is>
-          <t>P. Deb, A. Orr, D. H. Bromwich, J. P. Nicolas, J. Turner, J. S. Hosking</t>
+          <t>J. Turner, T. Phillips, M. Thamban, W. Rahaman, G. J. Marshall, J. D. Wille, V. Favier, V. H. Winton, E. Thomas, Z. Wang, M. Broeke, J. S. Hosking, T. Lachlan-Cope</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>10.1029/2018GL077092</t>
+          <t>10.1029/2018GL081517</t>
         </is>
       </c>
       <c r="D40" t="inlineStr"/>
@@ -2620,16 +2620,20 @@
         </is>
       </c>
       <c r="G40" t="inlineStr"/>
-      <c r="H40" t="inlineStr"/>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>Phys.org, black, https://phys.org/news/2019-03-antarctic-snowfall-dominated-extreme-snowstorms.html</t>
+        </is>
+      </c>
       <c r="I40" t="inlineStr"/>
       <c r="J40" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>6</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>4124-4133</t>
+          <t>3502-3511</t>
         </is>
       </c>
       <c r="L40" t="inlineStr"/>
@@ -2637,7 +2641,7 @@
       <c r="N40" t="inlineStr"/>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Summer Drivers of Atmospheric Variability Affecting Ice Shelf Thinning in the Amundsen Sea Embayment, West Antarctica</t>
+          <t>The Dominant Role of Extreme Precipitation Events in Antarctic Snowfall Variability</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
@@ -2645,15 +2649,19 @@
           <t>article</t>
         </is>
       </c>
-      <c r="Q40" t="inlineStr"/>
+      <c r="Q40" t="inlineStr">
+        <is>
+          <t>https://agupubs.onlinelibrary.wiley.com/doi/abs/10.1029/2018GL081517</t>
+        </is>
+      </c>
       <c r="R40" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>46</t>
         </is>
       </c>
       <c r="S40" t="inlineStr">
         <is>
-          <t>2018</t>
+          <t>2019</t>
         </is>
       </c>
     </row>
@@ -2661,36 +2669,32 @@
       <c r="A41" t="inlineStr"/>
       <c r="B41" t="inlineStr">
         <is>
-          <t>J. S. Hosking, D. MacLeod, T. Phillips, C. R. Holmes, P. Watson, E. Shuckburgh, D. Mitchell</t>
+          <t>P. Deb, A. Orr, D. H. Bromwich, J. P. Nicolas, J. Turner, J. S. Hosking</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>10.1088/1748-9326/aabf78</t>
+          <t>10.1029/2018GL077092</t>
         </is>
       </c>
       <c r="D41" t="inlineStr"/>
       <c r="E41" t="inlineStr"/>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Environmental Research Letters</t>
+          <t>Geophysical Research Letters</t>
         </is>
       </c>
       <c r="G41" t="inlineStr"/>
-      <c r="H41" t="inlineStr">
-        <is>
-          <t>Carbon Brief, blue, https://www.carbonbrief.org/uk-onshore-wind-energy-potential-could-rise-by-10-with-1-5c-warming; Independent, red, https://www.independent.co.uk/climate-change/news/wind-power-uk-global-warming-climate-change-british-antarctic-survey-a8354956.html; Phys.org, black, https://phys.org/news/2018-05-european-energy-potential-degree-warmer.html; Mail Online, DarkOrange, https://www.dailymail.co.uk/sciencetech/article-5736189/Global-warming-make-UK-large-parts-northern-Europe-far-windier.html; Treehugger, green, https://www.treehugger.com/climate-change-could-bring-stronger-winds-more-wind-power-4857464</t>
-        </is>
-      </c>
+      <c r="H41" t="inlineStr"/>
       <c r="I41" t="inlineStr"/>
       <c r="J41" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>9</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>1--9</t>
+          <t>4124-4133</t>
         </is>
       </c>
       <c r="L41" t="inlineStr"/>
@@ -2698,7 +2702,7 @@
       <c r="N41" t="inlineStr"/>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Changes in European wind energy generation potential within a 1.5C warmer world</t>
+          <t>Summer Drivers of Atmospheric Variability Affecting Ice Shelf Thinning in the Amundsen Sea Embayment, West Antarctica</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
@@ -2709,7 +2713,7 @@
       <c r="Q41" t="inlineStr"/>
       <c r="R41" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>45</t>
         </is>
       </c>
       <c r="S41" t="inlineStr">
@@ -2722,32 +2726,36 @@
       <c r="A42" t="inlineStr"/>
       <c r="B42" t="inlineStr">
         <is>
-          <t>J. C. King, D. Bannister, J. S. Hosking, S. R. Colwell</t>
+          <t>J. S. Hosking, D. MacLeod, T. Phillips, C. R. Holmes, P. Watson, E. Shuckburgh, D. Mitchell</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>10.1002/asl.793</t>
+          <t>10.1088/1748-9326/aabf78</t>
         </is>
       </c>
       <c r="D42" t="inlineStr"/>
       <c r="E42" t="inlineStr"/>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Atmospheric Science Letters</t>
+          <t>Environmental Research Letters</t>
         </is>
       </c>
       <c r="G42" t="inlineStr"/>
-      <c r="H42" t="inlineStr"/>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>Carbon Brief, blue, https://www.carbonbrief.org/uk-onshore-wind-energy-potential-could-rise-by-10-with-1-5c-warming; Independent, red, https://www.independent.co.uk/climate-change/news/wind-power-uk-global-warming-climate-change-british-antarctic-survey-a8354956.html; Phys.org, black, https://phys.org/news/2018-05-european-energy-potential-degree-warmer.html; Mail Online, DarkOrange, https://www.dailymail.co.uk/sciencetech/article-5736189/Global-warming-make-UK-large-parts-northern-Europe-far-windier.html; Treehugger, green, https://www.treehugger.com/climate-change-could-bring-stronger-winds-more-wind-power-4857464</t>
+        </is>
+      </c>
       <c r="I42" t="inlineStr"/>
       <c r="J42" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>5</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>491-496</t>
+          <t>1--9</t>
         </is>
       </c>
       <c r="L42" t="inlineStr"/>
@@ -2755,7 +2763,7 @@
       <c r="N42" t="inlineStr"/>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Causes of the Antarctic region record high temperature at Signy Island, 30th January 1982</t>
+          <t>Changes in European wind energy generation potential within a 1.5C warmer world</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
@@ -2766,12 +2774,12 @@
       <c r="Q42" t="inlineStr"/>
       <c r="R42" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>13</t>
         </is>
       </c>
       <c r="S42" t="inlineStr">
         <is>
-          <t>2017</t>
+          <t>2018</t>
         </is>
       </c>
     </row>
@@ -2779,19 +2787,19 @@
       <c r="A43" t="inlineStr"/>
       <c r="B43" t="inlineStr">
         <is>
-          <t>J. S. Hosking, R. Fogt, E. R. Thomas, V. Moosavi, T. Phillips, J. Coggins, D. Reusch</t>
+          <t>J. C. King, D. Bannister, J. S. Hosking, S. R. Colwell</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>10.1002/2017GL074722</t>
+          <t>10.1002/asl.793</t>
         </is>
       </c>
       <c r="D43" t="inlineStr"/>
       <c r="E43" t="inlineStr"/>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Geophysical Research Letters</t>
+          <t>Atmospheric Science Letters</t>
         </is>
       </c>
       <c r="G43" t="inlineStr"/>
@@ -2799,12 +2807,12 @@
       <c r="I43" t="inlineStr"/>
       <c r="J43" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>12</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>9084-9092</t>
+          <t>491-496</t>
         </is>
       </c>
       <c r="L43" t="inlineStr"/>
@@ -2812,7 +2820,7 @@
       <c r="N43" t="inlineStr"/>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Accumulation in coastal West Antarctic ice core records and the role of cyclone activity</t>
+          <t>Causes of the Antarctic region record high temperature at Signy Island, 30th January 1982</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
@@ -2823,7 +2831,7 @@
       <c r="Q43" t="inlineStr"/>
       <c r="R43" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>18</t>
         </is>
       </c>
       <c r="S43" t="inlineStr">
@@ -2836,19 +2844,19 @@
       <c r="A44" t="inlineStr"/>
       <c r="B44" t="inlineStr">
         <is>
-          <t>D. Bannister, M. Herzog, H.-F. Graf, J. S. Hosking, C. A. Short</t>
+          <t>J. S. Hosking, R. Fogt, E. R. Thomas, V. Moosavi, T. Phillips, J. Coggins, D. Reusch</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>10.1175/JCLI-D-16-0536.1</t>
+          <t>10.1002/2017GL074722</t>
         </is>
       </c>
       <c r="D44" t="inlineStr"/>
       <c r="E44" t="inlineStr"/>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Journal of Climate</t>
+          <t>Geophysical Research Letters</t>
         </is>
       </c>
       <c r="G44" t="inlineStr"/>
@@ -2861,7 +2869,7 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>6701-6722</t>
+          <t>9084-9092</t>
         </is>
       </c>
       <c r="L44" t="inlineStr"/>
@@ -2869,7 +2877,7 @@
       <c r="N44" t="inlineStr"/>
       <c r="O44" t="inlineStr">
         <is>
-          <t>An Assessment of Recent and Future Temperature Change over the Sichuan Basin, China, Using CMIP5 Climate Models</t>
+          <t>Accumulation in coastal West Antarctic ice core records and the role of cyclone activity</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
@@ -2880,7 +2888,7 @@
       <c r="Q44" t="inlineStr"/>
       <c r="R44" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>44</t>
         </is>
       </c>
       <c r="S44" t="inlineStr">
@@ -2893,36 +2901,32 @@
       <c r="A45" t="inlineStr"/>
       <c r="B45" t="inlineStr">
         <is>
-          <t>J. Turner, T. Phillips, G. J. Marshall, J. S. Hosking, J. O. Pope, T. J. Bracegirdle, P. Deb</t>
+          <t>D. Bannister, M. Herzog, H.-F. Graf, J. S. Hosking, C. A. Short</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>10.1002/2017GL073656</t>
+          <t>10.1175/JCLI-D-16-0536.1</t>
         </is>
       </c>
       <c r="D45" t="inlineStr"/>
       <c r="E45" t="inlineStr"/>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Geophysical Research Letters</t>
+          <t>Journal of Climate</t>
         </is>
       </c>
       <c r="G45" t="inlineStr"/>
-      <c r="H45" t="inlineStr">
-        <is>
-          <t>Phys.org, black, https://phys.org/news/2017-06-storms-massive-antarctic-sea-ice.html</t>
-        </is>
-      </c>
+      <c r="H45" t="inlineStr"/>
       <c r="I45" t="inlineStr"/>
       <c r="J45" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>17</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>6868--6875</t>
+          <t>6701-6722</t>
         </is>
       </c>
       <c r="L45" t="inlineStr"/>
@@ -2930,7 +2934,7 @@
       <c r="N45" t="inlineStr"/>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Unprecedented springtime retreat of Antarctic sea ice in 2016</t>
+          <t>An Assessment of Recent and Future Temperature Change over the Sichuan Basin, China, Using CMIP5 Climate Models</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
@@ -2941,7 +2945,7 @@
       <c r="Q45" t="inlineStr"/>
       <c r="R45" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>30</t>
         </is>
       </c>
       <c r="S45" t="inlineStr">
@@ -2954,32 +2958,36 @@
       <c r="A46" t="inlineStr"/>
       <c r="B46" t="inlineStr">
         <is>
-          <t>T. Moffat-Griffin, M. J. Taylor, T. Nakamura, A. J. Kavanagh, J. S. Hosking, A. Orr</t>
+          <t>J. Turner, T. Phillips, G. J. Marshall, J. S. Hosking, J. O. Pope, T. J. Bracegirdle, P. Deb</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>10.1007/s00376-016-6197-5</t>
+          <t>10.1002/2017GL073656</t>
         </is>
       </c>
       <c r="D46" t="inlineStr"/>
       <c r="E46" t="inlineStr"/>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Advances in Atmospheric Sciences</t>
+          <t>Geophysical Research Letters</t>
         </is>
       </c>
       <c r="G46" t="inlineStr"/>
-      <c r="H46" t="inlineStr"/>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>Phys.org, black, https://phys.org/news/2017-06-storms-massive-antarctic-sea-ice.html</t>
+        </is>
+      </c>
       <c r="I46" t="inlineStr"/>
       <c r="J46" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>13</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>1--3</t>
+          <t>6868--6875</t>
         </is>
       </c>
       <c r="L46" t="inlineStr"/>
@@ -2987,7 +2995,7 @@
       <c r="N46" t="inlineStr"/>
       <c r="O46" t="inlineStr">
         <is>
-          <t>3rd ANtarctic Gravity Wave Instrument Network (ANGWIN) science workshop</t>
+          <t>Unprecedented springtime retreat of Antarctic sea ice in 2016</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
@@ -2998,7 +3006,7 @@
       <c r="Q46" t="inlineStr"/>
       <c r="R46" t="inlineStr">
         <is>
-          <t>34</t>
+          <t>44</t>
         </is>
       </c>
       <c r="S46" t="inlineStr">
@@ -3011,19 +3019,19 @@
       <c r="A47" t="inlineStr"/>
       <c r="B47" t="inlineStr">
         <is>
-          <t>J. Turner, J. S. Hosking, T. J. Bracegirdle, T. Phillips, G. J. Marshall</t>
+          <t>T. Moffat-Griffin, M. J. Taylor, T. Nakamura, A. J. Kavanagh, J. S. Hosking, A. Orr</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>10.1002/joc.4848</t>
+          <t>10.1007/s00376-016-6197-5</t>
         </is>
       </c>
       <c r="D47" t="inlineStr"/>
       <c r="E47" t="inlineStr"/>
       <c r="F47" t="inlineStr">
         <is>
-          <t>International Journal of Climatology</t>
+          <t>Advances in Atmospheric Sciences</t>
         </is>
       </c>
       <c r="G47" t="inlineStr"/>
@@ -3031,12 +3039,12 @@
       <c r="I47" t="inlineStr"/>
       <c r="J47" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>2325--2336</t>
+          <t>1--3</t>
         </is>
       </c>
       <c r="L47" t="inlineStr"/>
@@ -3044,7 +3052,7 @@
       <c r="N47" t="inlineStr"/>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Variability and trends in the Southern Hemisphere high latitude, quasi-stationary planetary waves</t>
+          <t>3rd ANtarctic Gravity Wave Instrument Network (ANGWIN) science workshop</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
@@ -3055,7 +3063,7 @@
       <c r="Q47" t="inlineStr"/>
       <c r="R47" t="inlineStr">
         <is>
-          <t>37</t>
+          <t>34</t>
         </is>
       </c>
       <c r="S47" t="inlineStr">
@@ -3068,32 +3076,32 @@
       <c r="A48" t="inlineStr"/>
       <c r="B48" t="inlineStr">
         <is>
-          <t>J. Turner, H. Lu, I. White, J. King, T. Phillips, J. S. Hosking, T. J. Bracegirdle, G. J. Marshall, R. Mulvaney, P. Deb</t>
+          <t>J. Turner, J. S. Hosking, T. J. Bracegirdle, T. Phillips, G. J. Marshall</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>10.1038/nature18645</t>
+          <t>10.1002/joc.4848</t>
         </is>
       </c>
       <c r="D48" t="inlineStr"/>
       <c r="E48" t="inlineStr"/>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Nature</t>
+          <t>International Journal of Climatology</t>
         </is>
       </c>
       <c r="G48" t="inlineStr"/>
-      <c r="H48" t="inlineStr">
-        <is>
-          <t>Carbon Brief, blue, https://www.carbonbrief.org/natural-forces-overpowering-antarctic-peninsula-warming; Washington Post, black, https://www.washingtonpost.com/news/energy-environment/wp/2016/07/20/the-antarctic-peninsula-is-cooling-but-climate-skeptics-shouldnt-get-too-excited/</t>
-        </is>
-      </c>
+      <c r="H48" t="inlineStr"/>
       <c r="I48" t="inlineStr"/>
-      <c r="J48" t="inlineStr"/>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>411--415</t>
+          <t>2325--2336</t>
         </is>
       </c>
       <c r="L48" t="inlineStr"/>
@@ -3101,7 +3109,7 @@
       <c r="N48" t="inlineStr"/>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Absence of 21st century warming on Antarctic Peninsula consistent with natural variability</t>
+          <t>Variability and trends in the Southern Hemisphere high latitude, quasi-stationary planetary waves</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
@@ -3112,12 +3120,12 @@
       <c r="Q48" t="inlineStr"/>
       <c r="R48" t="inlineStr">
         <is>
-          <t>535</t>
+          <t>37</t>
         </is>
       </c>
       <c r="S48" t="inlineStr">
         <is>
-          <t>2016</t>
+          <t>2017</t>
         </is>
       </c>
     </row>
@@ -3125,32 +3133,32 @@
       <c r="A49" t="inlineStr"/>
       <c r="B49" t="inlineStr">
         <is>
-          <t>P. Deb, A. Orr, J. S. Hosking, T. Phillips, J. Turner, D. Bannister, J. O. Pope, S. Colwell</t>
+          <t>J. Turner, H. Lu, I. White, J. King, T. Phillips, J. S. Hosking, T. J. Bracegirdle, G. J. Marshall, R. Mulvaney, P. Deb</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>10.1002/2015JD024037</t>
+          <t>10.1038/nature18645</t>
         </is>
       </c>
       <c r="D49" t="inlineStr"/>
       <c r="E49" t="inlineStr"/>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Journal of Geophysical Research: Atmospheres</t>
+          <t>Nature</t>
         </is>
       </c>
       <c r="G49" t="inlineStr"/>
-      <c r="H49" t="inlineStr"/>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>Carbon Brief, blue, https://www.carbonbrief.org/natural-forces-overpowering-antarctic-peninsula-warming; Washington Post, black, https://www.washingtonpost.com/news/energy-environment/wp/2016/07/20/the-antarctic-peninsula-is-cooling-but-climate-skeptics-shouldnt-get-too-excited/</t>
+        </is>
+      </c>
       <c r="I49" t="inlineStr"/>
-      <c r="J49" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
+      <c r="J49" t="inlineStr"/>
       <c r="K49" t="inlineStr">
         <is>
-          <t>1532-1548</t>
+          <t>411--415</t>
         </is>
       </c>
       <c r="L49" t="inlineStr"/>
@@ -3158,7 +3166,7 @@
       <c r="N49" t="inlineStr"/>
       <c r="O49" t="inlineStr">
         <is>
-          <t>An assessment of the Polar Weather Research and Forecasting (WRF) model representation of near-surface meteorological variables over West Antarctica</t>
+          <t>Absence of 21st century warming on Antarctic Peninsula consistent with natural variability</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
@@ -3169,7 +3177,7 @@
       <c r="Q49" t="inlineStr"/>
       <c r="R49" t="inlineStr">
         <is>
-          <t>121</t>
+          <t>535</t>
         </is>
       </c>
       <c r="S49" t="inlineStr">
@@ -3182,19 +3190,19 @@
       <c r="A50" t="inlineStr"/>
       <c r="B50" t="inlineStr">
         <is>
-          <t>J. S. Hosking, A. Orr, T. J. Bracegirdle, J. Turner</t>
+          <t>P. Deb, A. Orr, J. S. Hosking, T. Phillips, J. Turner, D. Bannister, J. O. Pope, S. Colwell</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>10.1002/2015GL067143</t>
+          <t>10.1002/2015JD024037</t>
         </is>
       </c>
       <c r="D50" t="inlineStr"/>
       <c r="E50" t="inlineStr"/>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Geophysical Research Letters</t>
+          <t>Journal of Geophysical Research: Atmospheres</t>
         </is>
       </c>
       <c r="G50" t="inlineStr"/>
@@ -3202,12 +3210,12 @@
       <c r="I50" t="inlineStr"/>
       <c r="J50" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>367-376</t>
+          <t>1532-1548</t>
         </is>
       </c>
       <c r="L50" t="inlineStr"/>
@@ -3215,7 +3223,7 @@
       <c r="N50" t="inlineStr"/>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Future circulation changes off West Antarctica: Sensitivity of the Amundsen Sea Low to projected anthropogenic forcing</t>
+          <t>An assessment of the Polar Weather Research and Forecasting (WRF) model representation of near-surface meteorological variables over West Antarctica</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
@@ -3226,7 +3234,7 @@
       <c r="Q50" t="inlineStr"/>
       <c r="R50" t="inlineStr">
         <is>
-          <t>43</t>
+          <t>121</t>
         </is>
       </c>
       <c r="S50" t="inlineStr">
@@ -3239,19 +3247,19 @@
       <c r="A51" t="inlineStr"/>
       <c r="B51" t="inlineStr">
         <is>
-          <t>M. N. Raphael, G. J. Marshall, J. Turner, R. L. Fogt, D. Schneider, D. A. Dixon, J. S. Hosking, J. M. Jones, W. R. Hobbs</t>
+          <t>J. S. Hosking, A. Orr, T. J. Bracegirdle, J. Turner</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>10.1175/BAMS-D-14-00018.1</t>
+          <t>10.1002/2015GL067143</t>
         </is>
       </c>
       <c r="D51" t="inlineStr"/>
       <c r="E51" t="inlineStr"/>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Bulletin of the American Meteorological Society</t>
+          <t>Geophysical Research Letters</t>
         </is>
       </c>
       <c r="G51" t="inlineStr"/>
@@ -3264,7 +3272,7 @@
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>111-121</t>
+          <t>367-376</t>
         </is>
       </c>
       <c r="L51" t="inlineStr"/>
@@ -3272,7 +3280,7 @@
       <c r="N51" t="inlineStr"/>
       <c r="O51" t="inlineStr">
         <is>
-          <t>The Amundsen Sea Low: Variability, Change, and Impact on Antarctic Climate</t>
+          <t>Future circulation changes off West Antarctica: Sensitivity of the Amundsen Sea Low to projected anthropogenic forcing</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
@@ -3283,7 +3291,7 @@
       <c r="Q51" t="inlineStr"/>
       <c r="R51" t="inlineStr">
         <is>
-          <t>97</t>
+          <t>43</t>
         </is>
       </c>
       <c r="S51" t="inlineStr">
@@ -3296,19 +3304,19 @@
       <c r="A52" t="inlineStr"/>
       <c r="B52" t="inlineStr">
         <is>
-          <t>J. Turner, J. S. Hosking, G. J. Marshall, T. Phillips, T. J. Bracegirdle</t>
+          <t>M. N. Raphael, G. J. Marshall, J. Turner, R. L. Fogt, D. Schneider, D. A. Dixon, J. S. Hosking, J. M. Jones, W. R. Hobbs</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>10.1007/s00382-015-2708-9</t>
+          <t>10.1175/BAMS-D-14-00018.1</t>
         </is>
       </c>
       <c r="D52" t="inlineStr"/>
       <c r="E52" t="inlineStr"/>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Climate Dynamics</t>
+          <t>Bulletin of the American Meteorological Society</t>
         </is>
       </c>
       <c r="G52" t="inlineStr"/>
@@ -3316,12 +3324,12 @@
       <c r="I52" t="inlineStr"/>
       <c r="J52" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>2391--2402</t>
+          <t>111-121</t>
         </is>
       </c>
       <c r="L52" t="inlineStr"/>
@@ -3329,7 +3337,7 @@
       <c r="N52" t="inlineStr"/>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Antarctic sea ice increase dominated by intrinsic variability of the Amundsen Sea Low</t>
+          <t>The Amundsen Sea Low: Variability, Change, and Impact on Antarctic Climate</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
@@ -3340,7 +3348,7 @@
       <c r="Q52" t="inlineStr"/>
       <c r="R52" t="inlineStr">
         <is>
-          <t>46</t>
+          <t>97</t>
         </is>
       </c>
       <c r="S52" t="inlineStr">
@@ -3353,36 +3361,32 @@
       <c r="A53" t="inlineStr"/>
       <c r="B53" t="inlineStr">
         <is>
-          <t>E. R. Thomas, J. S. Hosking, R. R. Tuckwell, R. A. Warren, E. C. Ludlow</t>
+          <t>J. Turner, J. S. Hosking, G. J. Marshall, T. Phillips, T. J. Bracegirdle</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>10.1002/2015GL065750</t>
+          <t>10.1007/s00382-015-2708-9</t>
         </is>
       </c>
       <c r="D53" t="inlineStr"/>
       <c r="E53" t="inlineStr"/>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Geophysical Research Letters</t>
+          <t>Climate Dynamics</t>
         </is>
       </c>
       <c r="G53" t="inlineStr"/>
-      <c r="H53" t="inlineStr">
-        <is>
-          <t>Indian Express, red, https://indianexpress.com/article/trending/trending-globally/west-antarctic-coastal-snow-rose-30-per-cent-in-20th-century/</t>
-        </is>
-      </c>
+      <c r="H53" t="inlineStr"/>
       <c r="I53" t="inlineStr"/>
       <c r="J53" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>7</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
         <is>
-          <t>9387--9393</t>
+          <t>2391--2402</t>
         </is>
       </c>
       <c r="L53" t="inlineStr"/>
@@ -3390,7 +3394,7 @@
       <c r="N53" t="inlineStr"/>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Twentieth century increase in snowfall in coastal West Antarctica</t>
+          <t>Antarctic sea ice increase dominated by intrinsic variability of the Amundsen Sea Low</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
@@ -3401,12 +3405,12 @@
       <c r="Q53" t="inlineStr"/>
       <c r="R53" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>46</t>
         </is>
       </c>
       <c r="S53" t="inlineStr">
         <is>
-          <t>2015</t>
+          <t>2016</t>
         </is>
       </c>
     </row>
@@ -3414,36 +3418,44 @@
       <c r="A54" t="inlineStr"/>
       <c r="B54" t="inlineStr">
         <is>
-          <t>J. Turner, J. S. Hosking, T. J. Bracegirdle, G. J. Marshall, T. Phillips</t>
+          <t>E. R. Thomas, J. S. Hosking, R. R. Tuckwell, R. A. Warren, E. C. Ludlow</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>10.1098/rsta.2014.0163</t>
+          <t>10.1002/2015GL065750</t>
         </is>
       </c>
       <c r="D54" t="inlineStr"/>
       <c r="E54" t="inlineStr"/>
       <c r="F54" t="inlineStr">
         <is>
-          <t>Philosophical Transactions of the Royal Society of London A: Mathematical, Physical and Engineering Sciences</t>
+          <t>Geophysical Research Letters</t>
         </is>
       </c>
       <c r="G54" t="inlineStr"/>
-      <c r="H54" t="inlineStr"/>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>Indian Express, red, https://indianexpress.com/article/trending/trending-globally/west-antarctic-coastal-snow-rose-30-per-cent-in-20th-century/</t>
+        </is>
+      </c>
       <c r="I54" t="inlineStr"/>
       <c r="J54" t="inlineStr">
         <is>
-          <t>2045</t>
-        </is>
-      </c>
-      <c r="K54" t="inlineStr"/>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>9387--9393</t>
+        </is>
+      </c>
       <c r="L54" t="inlineStr"/>
       <c r="M54" t="inlineStr"/>
       <c r="N54" t="inlineStr"/>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Recent Changes in Antarctic Sea Ice</t>
+          <t>Twentieth century increase in snowfall in coastal West Antarctica</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
@@ -3454,7 +3466,7 @@
       <c r="Q54" t="inlineStr"/>
       <c r="R54" t="inlineStr">
         <is>
-          <t>373</t>
+          <t>42</t>
         </is>
       </c>
       <c r="S54" t="inlineStr">
@@ -3467,19 +3479,19 @@
       <c r="A55" t="inlineStr"/>
       <c r="B55" t="inlineStr">
         <is>
-          <t>C. Chemel, M. R. Russo, J. S. Hosking, P. J. Telford, J. A. Pyle</t>
+          <t>J. Turner, J. S. Hosking, T. J. Bracegirdle, G. J. Marshall, T. Phillips</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>10.1002/asl2.540</t>
+          <t>10.1098/rsta.2014.0163</t>
         </is>
       </c>
       <c r="D55" t="inlineStr"/>
       <c r="E55" t="inlineStr"/>
       <c r="F55" t="inlineStr">
         <is>
-          <t>Atmospheric Science Letters</t>
+          <t>Philosophical Transactions of the Royal Society of London A: Mathematical, Physical and Engineering Sciences</t>
         </is>
       </c>
       <c r="G55" t="inlineStr"/>
@@ -3487,20 +3499,16 @@
       <c r="I55" t="inlineStr"/>
       <c r="J55" t="inlineStr">
         <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="K55" t="inlineStr">
-        <is>
-          <t>148-154</t>
-        </is>
-      </c>
+          <t>2045</t>
+        </is>
+      </c>
+      <c r="K55" t="inlineStr"/>
       <c r="L55" t="inlineStr"/>
       <c r="M55" t="inlineStr"/>
       <c r="N55" t="inlineStr"/>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Sensitivity of tropical deep convection in global models: effects of horizontal resolution, surface constraints and 3D atmospheric nudging</t>
+          <t>Recent Changes in Antarctic Sea Ice</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
@@ -3511,7 +3519,7 @@
       <c r="Q55" t="inlineStr"/>
       <c r="R55" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>373</t>
         </is>
       </c>
       <c r="S55" t="inlineStr">
@@ -3524,19 +3532,19 @@
       <c r="A56" t="inlineStr"/>
       <c r="B56" t="inlineStr">
         <is>
-          <t>A. Orr, J. S. Hosking, L. Hoffmann, J. Keeble, S. M. Dean, H. K. Roscoe, N. L. Abraham, S. Vosper, P. Braesicke</t>
+          <t>C. Chemel, M. R. Russo, J. S. Hosking, P. J. Telford, J. A. Pyle</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>10.5194/acp-15-1071-2015</t>
+          <t>10.1002/asl2.540</t>
         </is>
       </c>
       <c r="D56" t="inlineStr"/>
       <c r="E56" t="inlineStr"/>
       <c r="F56" t="inlineStr">
         <is>
-          <t>Atmospheric Chemistry and Physics</t>
+          <t>Atmospheric Science Letters</t>
         </is>
       </c>
       <c r="G56" t="inlineStr"/>
@@ -3549,7 +3557,7 @@
       </c>
       <c r="K56" t="inlineStr">
         <is>
-          <t>1071--1086</t>
+          <t>148-154</t>
         </is>
       </c>
       <c r="L56" t="inlineStr"/>
@@ -3557,7 +3565,7 @@
       <c r="N56" t="inlineStr"/>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Inclusion of mountain-wave-induced cooling for the formation of PSCs over the Antarctic Peninsula in a chemistry-climate model</t>
+          <t>Sensitivity of tropical deep convection in global models: effects of horizontal resolution, surface constraints and 3D atmospheric nudging</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
@@ -3568,7 +3576,7 @@
       <c r="Q56" t="inlineStr"/>
       <c r="R56" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>16</t>
         </is>
       </c>
       <c r="S56" t="inlineStr">
@@ -3581,19 +3589,19 @@
       <c r="A57" t="inlineStr"/>
       <c r="B57" t="inlineStr">
         <is>
-          <t>J. S. Hosking, D. Bannister, A. Orr, J. King, E. Young, T. Phillips</t>
+          <t>A. Orr, J. S. Hosking, L. Hoffmann, J. Keeble, S. M. Dean, H. K. Roscoe, N. L. Abraham, S. Vosper, P. Braesicke</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>10.1002/asl2.519</t>
+          <t>10.5194/acp-15-1071-2015</t>
         </is>
       </c>
       <c r="D57" t="inlineStr"/>
       <c r="E57" t="inlineStr"/>
       <c r="F57" t="inlineStr">
         <is>
-          <t>Atmospheric Science Letters</t>
+          <t>Atmospheric Chemistry and Physics</t>
         </is>
       </c>
       <c r="G57" t="inlineStr"/>
@@ -3601,12 +3609,12 @@
       <c r="I57" t="inlineStr"/>
       <c r="J57" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="K57" t="inlineStr">
         <is>
-          <t>50-55</t>
+          <t>1071--1086</t>
         </is>
       </c>
       <c r="L57" t="inlineStr"/>
@@ -3614,7 +3622,7 @@
       <c r="N57" t="inlineStr"/>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Orographic disturbances of surface winds over the shelf waters adjacent to South Georgia</t>
+          <t>Inclusion of mountain-wave-induced cooling for the formation of PSCs over the Antarctic Peninsula in a chemistry-climate model</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
@@ -3625,7 +3633,7 @@
       <c r="Q57" t="inlineStr"/>
       <c r="R57" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>15</t>
         </is>
       </c>
       <c r="S57" t="inlineStr">
@@ -3638,19 +3646,19 @@
       <c r="A58" t="inlineStr"/>
       <c r="B58" t="inlineStr">
         <is>
-          <t>A. Orr, T. Phillips, S. Webster, A. Elvidge, M. Weeks, S. Hosking, J. Turner</t>
+          <t>J. S. Hosking, D. Bannister, A. Orr, J. King, E. Young, T. Phillips</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>10.1002/qj.2296</t>
+          <t>10.1002/asl2.519</t>
         </is>
       </c>
       <c r="D58" t="inlineStr"/>
       <c r="E58" t="inlineStr"/>
       <c r="F58" t="inlineStr">
         <is>
-          <t>Quarterly Journal of the Royal Meteorological Society</t>
+          <t>Atmospheric Science Letters</t>
         </is>
       </c>
       <c r="G58" t="inlineStr"/>
@@ -3658,12 +3666,12 @@
       <c r="I58" t="inlineStr"/>
       <c r="J58" t="inlineStr">
         <is>
-          <t>684</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K58" t="inlineStr">
         <is>
-          <t>2287-2297</t>
+          <t>50-55</t>
         </is>
       </c>
       <c r="L58" t="inlineStr"/>
@@ -3671,7 +3679,7 @@
       <c r="N58" t="inlineStr"/>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Met Office Unified Model high resolution simulations of a strong wind event in Antarctica</t>
+          <t>Orographic disturbances of surface winds over the shelf waters adjacent to South Georgia</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
@@ -3682,12 +3690,12 @@
       <c r="Q58" t="inlineStr"/>
       <c r="R58" t="inlineStr">
         <is>
-          <t>140</t>
+          <t>16</t>
         </is>
       </c>
       <c r="S58" t="inlineStr">
         <is>
-          <t>2014</t>
+          <t>2015</t>
         </is>
       </c>
     </row>
@@ -3695,19 +3703,19 @@
       <c r="A59" t="inlineStr"/>
       <c r="B59" t="inlineStr">
         <is>
-          <t>T. Bracegirdle, J. Turner, J. S. Hosking, T. Phillips</t>
+          <t>A. Orr, T. Phillips, S. Webster, A. Elvidge, M. Weeks, S. Hosking, J. Turner</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>10.1007/s00382-013-2032-1</t>
+          <t>10.1002/qj.2296</t>
         </is>
       </c>
       <c r="D59" t="inlineStr"/>
       <c r="E59" t="inlineStr"/>
       <c r="F59" t="inlineStr">
         <is>
-          <t>Climate Dynamics</t>
+          <t>Quarterly Journal of the Royal Meteorological Society</t>
         </is>
       </c>
       <c r="G59" t="inlineStr"/>
@@ -3715,12 +3723,12 @@
       <c r="I59" t="inlineStr"/>
       <c r="J59" t="inlineStr">
         <is>
-          <t>7-8</t>
+          <t>684</t>
         </is>
       </c>
       <c r="K59" t="inlineStr">
         <is>
-          <t>2093-2104</t>
+          <t>2287-2297</t>
         </is>
       </c>
       <c r="L59" t="inlineStr"/>
@@ -3728,7 +3736,7 @@
       <c r="N59" t="inlineStr"/>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Sources of uncertainty in projections of twenty-first century westerly wind changes over the Amundsen Sea, West Antarctica, in CMIP5 climate models</t>
+          <t>Met Office Unified Model high resolution simulations of a strong wind event in Antarctica</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
@@ -3739,7 +3747,7 @@
       <c r="Q59" t="inlineStr"/>
       <c r="R59" t="inlineStr">
         <is>
-          <t>43</t>
+          <t>140</t>
         </is>
       </c>
       <c r="S59" t="inlineStr">
@@ -3752,19 +3760,19 @@
       <c r="A60" t="inlineStr"/>
       <c r="B60" t="inlineStr">
         <is>
-          <t>J. Turner, J. S. Hosking, T. Phillips, G. J. Marshall</t>
+          <t>T. Bracegirdle, J. Turner, J. S. Hosking, T. Phillips</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>10.1002/2013GL058371</t>
+          <t>10.1007/s00382-013-2032-1</t>
         </is>
       </c>
       <c r="D60" t="inlineStr"/>
       <c r="E60" t="inlineStr"/>
       <c r="F60" t="inlineStr">
         <is>
-          <t>Geophysical Research Letters</t>
+          <t>Climate Dynamics</t>
         </is>
       </c>
       <c r="G60" t="inlineStr"/>
@@ -3772,12 +3780,12 @@
       <c r="I60" t="inlineStr"/>
       <c r="J60" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>7-8</t>
         </is>
       </c>
       <c r="K60" t="inlineStr">
         <is>
-          <t>5894-5898</t>
+          <t>2093-2104</t>
         </is>
       </c>
       <c r="L60" t="inlineStr"/>
@@ -3785,7 +3793,7 @@
       <c r="N60" t="inlineStr"/>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Temporal and spatial evolution of the Antarctic sea ice prior to the September 2012 record maximum extent</t>
+          <t>Sources of uncertainty in projections of twenty-first century westerly wind changes over the Amundsen Sea, West Antarctica, in CMIP5 climate models</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
@@ -3796,12 +3804,12 @@
       <c r="Q60" t="inlineStr"/>
       <c r="R60" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>43</t>
         </is>
       </c>
       <c r="S60" t="inlineStr">
         <is>
-          <t>2013</t>
+          <t>2014</t>
         </is>
       </c>
     </row>
@@ -3809,19 +3817,19 @@
       <c r="A61" t="inlineStr"/>
       <c r="B61" t="inlineStr">
         <is>
-          <t>J. S. Hosking, A. Orr, G. J. Marshall, J. Turner, T. Phillips</t>
+          <t>J. Turner, J. S. Hosking, T. Phillips, G. J. Marshall</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>10.1175/JCLI-D-12-00813.1</t>
+          <t>10.1002/2013GL058371</t>
         </is>
       </c>
       <c r="D61" t="inlineStr"/>
       <c r="E61" t="inlineStr"/>
       <c r="F61" t="inlineStr">
         <is>
-          <t>Journal of Climate</t>
+          <t>Geophysical Research Letters</t>
         </is>
       </c>
       <c r="G61" t="inlineStr"/>
@@ -3829,12 +3837,12 @@
       <c r="I61" t="inlineStr"/>
       <c r="J61" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>22</t>
         </is>
       </c>
       <c r="K61" t="inlineStr">
         <is>
-          <t>6633--6648</t>
+          <t>5894-5898</t>
         </is>
       </c>
       <c r="L61" t="inlineStr"/>
@@ -3842,7 +3850,7 @@
       <c r="N61" t="inlineStr"/>
       <c r="O61" t="inlineStr">
         <is>
-          <t>The influence of the Amundsen-Bellingshausen Seas Low on the climate of West Antarctica and its representation in coupled climate model simulations</t>
+          <t>Temporal and spatial evolution of the Antarctic sea ice prior to the September 2012 record maximum extent</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
@@ -3853,7 +3861,7 @@
       <c r="Q61" t="inlineStr"/>
       <c r="R61" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>40</t>
         </is>
       </c>
       <c r="S61" t="inlineStr">
@@ -3866,19 +3874,19 @@
       <c r="A62" t="inlineStr"/>
       <c r="B62" t="inlineStr">
         <is>
-          <t>J. Turner, T. Phillips, J. S. Hosking, G. J. Marshall, A. Orr</t>
+          <t>J. S. Hosking, A. Orr, G. J. Marshall, J. Turner, T. Phillips</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>10.1002/joc.3558</t>
+          <t>10.1175/JCLI-D-12-00813.1</t>
         </is>
       </c>
       <c r="D62" t="inlineStr"/>
       <c r="E62" t="inlineStr"/>
       <c r="F62" t="inlineStr">
         <is>
-          <t>International Journal of Climatology</t>
+          <t>Journal of Climate</t>
         </is>
       </c>
       <c r="G62" t="inlineStr"/>
@@ -3886,12 +3894,12 @@
       <c r="I62" t="inlineStr"/>
       <c r="J62" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>17</t>
         </is>
       </c>
       <c r="K62" t="inlineStr">
         <is>
-          <t>1818--1829</t>
+          <t>6633--6648</t>
         </is>
       </c>
       <c r="L62" t="inlineStr"/>
@@ -3899,7 +3907,7 @@
       <c r="N62" t="inlineStr"/>
       <c r="O62" t="inlineStr">
         <is>
-          <t>The Amundsen Sea Low</t>
+          <t>The influence of the Amundsen-Bellingshausen Seas Low on the climate of West Antarctica and its representation in coupled climate model simulations</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
@@ -3910,7 +3918,7 @@
       <c r="Q62" t="inlineStr"/>
       <c r="R62" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>26</t>
         </is>
       </c>
       <c r="S62" t="inlineStr">
@@ -3923,19 +3931,19 @@
       <c r="A63" t="inlineStr"/>
       <c r="B63" t="inlineStr">
         <is>
-          <t>N. E. Barrand, D. Vaughan, N. Steiner, M. Tedesco, P. Kuipers Munneke, M. Broeke, J. S. Hosking</t>
+          <t>J. Turner, T. Phillips, J. S. Hosking, G. J. Marshall, A. Orr</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>10.1029/2012JF002559</t>
+          <t>10.1002/joc.3558</t>
         </is>
       </c>
       <c r="D63" t="inlineStr"/>
       <c r="E63" t="inlineStr"/>
       <c r="F63" t="inlineStr">
         <is>
-          <t>Journal of Geophysical Research: Earth Surface</t>
+          <t>International Journal of Climatology</t>
         </is>
       </c>
       <c r="G63" t="inlineStr"/>
@@ -3943,12 +3951,12 @@
       <c r="I63" t="inlineStr"/>
       <c r="J63" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>7</t>
         </is>
       </c>
       <c r="K63" t="inlineStr">
         <is>
-          <t>315-330</t>
+          <t>1818--1829</t>
         </is>
       </c>
       <c r="L63" t="inlineStr"/>
@@ -3956,7 +3964,7 @@
       <c r="N63" t="inlineStr"/>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Trends in Antarctic Peninsula surface melting conditions from observations and regional climate modelling</t>
+          <t>The Amundsen Sea Low</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
@@ -3967,7 +3975,7 @@
       <c r="Q63" t="inlineStr"/>
       <c r="R63" t="inlineStr">
         <is>
-          <t>118</t>
+          <t>33</t>
         </is>
       </c>
       <c r="S63" t="inlineStr">
@@ -3980,19 +3988,19 @@
       <c r="A64" t="inlineStr"/>
       <c r="B64" t="inlineStr">
         <is>
-          <t>J. Turner, T. Bracegirdle, T. Phillips, G. J. Marshall, J. S. Hosking</t>
+          <t>N. E. Barrand, D. Vaughan, N. Steiner, M. Tedesco, P. Kuipers Munneke, M. Broeke, J. S. Hosking</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>10.1175/JCLI-D-12-00068.1</t>
+          <t>10.1029/2012JF002559</t>
         </is>
       </c>
       <c r="D64" t="inlineStr"/>
       <c r="E64" t="inlineStr"/>
       <c r="F64" t="inlineStr">
         <is>
-          <t>Journal of Climate</t>
+          <t>Journal of Geophysical Research: Earth Surface</t>
         </is>
       </c>
       <c r="G64" t="inlineStr"/>
@@ -4000,12 +4008,12 @@
       <c r="I64" t="inlineStr"/>
       <c r="J64" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K64" t="inlineStr">
         <is>
-          <t>1473--1484</t>
+          <t>315-330</t>
         </is>
       </c>
       <c r="L64" t="inlineStr"/>
@@ -4013,7 +4021,7 @@
       <c r="N64" t="inlineStr"/>
       <c r="O64" t="inlineStr">
         <is>
-          <t>An Initial Assessment of Antarctic Sea Ice Extent in the CMIP5 Models</t>
+          <t>Trends in Antarctic Peninsula surface melting conditions from observations and regional climate modelling</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
@@ -4024,7 +4032,7 @@
       <c r="Q64" t="inlineStr"/>
       <c r="R64" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>118</t>
         </is>
       </c>
       <c r="S64" t="inlineStr">
@@ -4037,12 +4045,12 @@
       <c r="A65" t="inlineStr"/>
       <c r="B65" t="inlineStr">
         <is>
-          <t>A. Orr, T. J. Bracegirdle, J. S. Hosking, W. Feng, H. K. Roscoe, J. D. Haigh</t>
+          <t>J. Turner, T. Bracegirdle, T. Phillips, G. J. Marshall, J. S. Hosking</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>10.1175/JCLI-D-12-00480.1</t>
+          <t>10.1175/JCLI-D-12-00068.1</t>
         </is>
       </c>
       <c r="D65" t="inlineStr"/>
@@ -4057,12 +4065,12 @@
       <c r="I65" t="inlineStr"/>
       <c r="J65" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="K65" t="inlineStr">
         <is>
-          <t>662--668</t>
+          <t>1473--1484</t>
         </is>
       </c>
       <c r="L65" t="inlineStr"/>
@@ -4070,7 +4078,7 @@
       <c r="N65" t="inlineStr"/>
       <c r="O65" t="inlineStr">
         <is>
-          <t>Strong dynamical modulation of the cooling of the polar stratosphere associated with the Antarctic ozone hole</t>
+          <t>An Initial Assessment of Antarctic Sea Ice Extent in the CMIP5 Models</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
@@ -4094,19 +4102,19 @@
       <c r="A66" t="inlineStr"/>
       <c r="B66" t="inlineStr">
         <is>
-          <t>A. Orr, T. J. Bracegirdle, J. S. Hosking, T. Jung, J. D. Haigh, T. Phillips, W. Feng</t>
+          <t>A. Orr, T. J. Bracegirdle, J. S. Hosking, W. Feng, H. K. Roscoe, J. D. Haigh</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>10.1175/JAS-D-11-0210.1</t>
+          <t>10.1175/JCLI-D-12-00480.1</t>
         </is>
       </c>
       <c r="D66" t="inlineStr"/>
       <c r="E66" t="inlineStr"/>
       <c r="F66" t="inlineStr">
         <is>
-          <t>Journal of the Atmospheric Sciences</t>
+          <t>Journal of Climate</t>
         </is>
       </c>
       <c r="G66" t="inlineStr"/>
@@ -4114,12 +4122,12 @@
       <c r="I66" t="inlineStr"/>
       <c r="J66" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>2</t>
         </is>
       </c>
       <c r="K66" t="inlineStr">
         <is>
-          <t>2917--2932</t>
+          <t>662--668</t>
         </is>
       </c>
       <c r="L66" t="inlineStr"/>
@@ -4127,7 +4135,7 @@
       <c r="N66" t="inlineStr"/>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Possible Dynamical Mechanisms for Southern Hemisphere Climate Change due to the Ozone Hole</t>
+          <t>Strong dynamical modulation of the cooling of the polar stratosphere associated with the Antarctic ozone hole</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
@@ -4138,12 +4146,12 @@
       <c r="Q66" t="inlineStr"/>
       <c r="R66" t="inlineStr">
         <is>
-          <t>69</t>
+          <t>26</t>
         </is>
       </c>
       <c r="S66" t="inlineStr">
         <is>
-          <t>2012</t>
+          <t>2013</t>
         </is>
       </c>
     </row>
@@ -4151,19 +4159,19 @@
       <c r="A67" t="inlineStr"/>
       <c r="B67" t="inlineStr">
         <is>
-          <t>J. S. Hosking, M. R. Russo, P. Braesicke, J. A. Pyle</t>
+          <t>A. Orr, T. J. Bracegirdle, J. S. Hosking, T. Jung, J. D. Haigh, T. Phillips, W. Feng</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>10.5194/acp-12-9791-2012</t>
+          <t>10.1175/JAS-D-11-0210.1</t>
         </is>
       </c>
       <c r="D67" t="inlineStr"/>
       <c r="E67" t="inlineStr"/>
       <c r="F67" t="inlineStr">
         <is>
-          <t>Atmospheric Chemistry and Physics</t>
+          <t>Journal of the Atmospheric Sciences</t>
         </is>
       </c>
       <c r="G67" t="inlineStr"/>
@@ -4171,12 +4179,12 @@
       <c r="I67" t="inlineStr"/>
       <c r="J67" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>10</t>
         </is>
       </c>
       <c r="K67" t="inlineStr">
         <is>
-          <t>9791--9797</t>
+          <t>2917--2932</t>
         </is>
       </c>
       <c r="L67" t="inlineStr"/>
@@ -4184,7 +4192,7 @@
       <c r="N67" t="inlineStr"/>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Tropical convective transport and the Walker circulation</t>
+          <t>Possible Dynamical Mechanisms for Southern Hemisphere Climate Change due to the Ozone Hole</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
@@ -4195,7 +4203,7 @@
       <c r="Q67" t="inlineStr"/>
       <c r="R67" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>69</t>
         </is>
       </c>
       <c r="S67" t="inlineStr">
@@ -4208,12 +4216,12 @@
       <c r="A68" t="inlineStr"/>
       <c r="B68" t="inlineStr">
         <is>
-          <t>C. R. Hoyle, V. Mar&amp;eacute;cal, M. R. Russo, G. Allen, J. Arteta, C. Chemel, M. P. Chipperfield, F. D'Amato, O. Dessens, W. Feng, J. F. Hamilton, N. R. Harris, J. S. Hosking, A. C. Lewis, O. Morgenstern, T. Peter, J. A. Pyle, T. Reddmann, N. A. Richards, P. J. Telford, W. Tian, S. Viciani, A. Volz-Thomas, O. Wild, X. Yang, G. Zeng</t>
+          <t>J. S. Hosking, M. R. Russo, P. Braesicke, J. A. Pyle</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>10.5194/acp-11-8103-2011</t>
+          <t>10.5194/acp-12-9791-2012</t>
         </is>
       </c>
       <c r="D68" t="inlineStr"/>
@@ -4228,12 +4236,12 @@
       <c r="I68" t="inlineStr"/>
       <c r="J68" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>20</t>
         </is>
       </c>
       <c r="K68" t="inlineStr">
         <is>
-          <t>8103--8131</t>
+          <t>9791--9797</t>
         </is>
       </c>
       <c r="L68" t="inlineStr"/>
@@ -4241,7 +4249,7 @@
       <c r="N68" t="inlineStr"/>
       <c r="O68" t="inlineStr">
         <is>
-          <t>Representation of tropical deep convection in atmospheric models - Part 2: Tracer transport</t>
+          <t>Tropical convective transport and the Walker circulation</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
@@ -4252,12 +4260,12 @@
       <c r="Q68" t="inlineStr"/>
       <c r="R68" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="S68" t="inlineStr">
         <is>
-          <t>2011</t>
+          <t>2012</t>
         </is>
       </c>
     </row>
@@ -4265,12 +4273,12 @@
       <c r="A69" t="inlineStr"/>
       <c r="B69" t="inlineStr">
         <is>
-          <t>M. R. Russo, V. Mar&amp;eacute;cal, C. R. Hoyle, J. Arteta, C. Chemel, M. P. Chipperfield, O. Dessens, W. Feng, J. S. Hosking, P. J. Telford, O. Wild, X. Yang, J. A. Pyle</t>
+          <t>C. R. Hoyle, V. Mar&amp;eacute;cal, M. R. Russo, G. Allen, J. Arteta, C. Chemel, M. P. Chipperfield, F. D'Amato, O. Dessens, W. Feng, J. F. Hamilton, N. R. Harris, J. S. Hosking, A. C. Lewis, O. Morgenstern, T. Peter, J. A. Pyle, T. Reddmann, N. A. Richards, P. J. Telford, W. Tian, S. Viciani, A. Volz-Thomas, O. Wild, X. Yang, G. Zeng</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>10.5194/acp-11-2765-2011</t>
+          <t>10.5194/acp-11-8103-2011</t>
         </is>
       </c>
       <c r="D69" t="inlineStr"/>
@@ -4285,12 +4293,12 @@
       <c r="I69" t="inlineStr"/>
       <c r="J69" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>15</t>
         </is>
       </c>
       <c r="K69" t="inlineStr">
         <is>
-          <t>2765--2786</t>
+          <t>8103--8131</t>
         </is>
       </c>
       <c r="L69" t="inlineStr"/>
@@ -4298,7 +4306,7 @@
       <c r="N69" t="inlineStr"/>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Representation of tropical deep convection in atmospheric models - Part 1: Meteorology and comparison with satellite observations</t>
+          <t>Representation of tropical deep convection in atmospheric models - Part 2: Tracer transport</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
@@ -4322,12 +4330,12 @@
       <c r="A70" t="inlineStr"/>
       <c r="B70" t="inlineStr">
         <is>
-          <t>J. S. Hosking, M. R. Russo, P. Braesicke, J. A. Pyle</t>
+          <t>M. R. Russo, V. Mar&amp;eacute;cal, C. R. Hoyle, J. Arteta, C. Chemel, M. P. Chipperfield, O. Dessens, W. Feng, J. S. Hosking, P. J. Telford, O. Wild, X. Yang, J. A. Pyle</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>10.5194/acp-10-11175-2010</t>
+          <t>10.5194/acp-11-2765-2011</t>
         </is>
       </c>
       <c r="D70" t="inlineStr"/>
@@ -4342,12 +4350,12 @@
       <c r="I70" t="inlineStr"/>
       <c r="J70" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>6</t>
         </is>
       </c>
       <c r="K70" t="inlineStr">
         <is>
-          <t>11175--11188</t>
+          <t>2765--2786</t>
         </is>
       </c>
       <c r="L70" t="inlineStr"/>
@@ -4355,7 +4363,7 @@
       <c r="N70" t="inlineStr"/>
       <c r="O70" t="inlineStr">
         <is>
-          <t>Modelling deep convection and its impacts on the tropical tropopause layer</t>
+          <t>Representation of tropical deep convection in atmospheric models - Part 1: Meteorology and comparison with satellite observations</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
@@ -4366,12 +4374,12 @@
       <c r="Q70" t="inlineStr"/>
       <c r="R70" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>11</t>
         </is>
       </c>
       <c r="S70" t="inlineStr">
         <is>
-          <t>2010</t>
+          <t>2011</t>
         </is>
       </c>
     </row>
@@ -4379,60 +4387,56 @@
       <c r="A71" t="inlineStr"/>
       <c r="B71" t="inlineStr">
         <is>
-          <t>A. Conner, S. Hosking, J. Lloyd, A. Rao, G. Shaddick, M. Sharan</t>
+          <t>J. S. Hosking, M. R. Russo, P. Braesicke, J. A. Pyle</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>10.5281/zenodo.7712969</t>
-        </is>
-      </c>
-      <c r="D71" t="inlineStr">
-        <is>
-          <t>The Alan Turing Institute</t>
-        </is>
-      </c>
+          <t>10.5194/acp-10-11175-2010</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr"/>
       <c r="E71" t="inlineStr"/>
-      <c r="F71" t="inlineStr"/>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>Atmospheric Chemistry and Physics</t>
+        </is>
+      </c>
       <c r="G71" t="inlineStr"/>
       <c r="H71" t="inlineStr"/>
-      <c r="I71" t="inlineStr">
-        <is>
-          <t>March</t>
-        </is>
-      </c>
-      <c r="J71" t="inlineStr"/>
-      <c r="K71" t="inlineStr"/>
-      <c r="L71" t="inlineStr">
-        <is>
-          <t>https://zenodo.org/record/7712969/files/turing_asg_whitepaper_climatechange.pdf</t>
-        </is>
-      </c>
-      <c r="M71" t="inlineStr">
-        <is>
-          <t>Zenodo</t>
-        </is>
-      </c>
+      <c r="I71" t="inlineStr"/>
+      <c r="J71" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="K71" t="inlineStr">
+        <is>
+          <t>11175--11188</t>
+        </is>
+      </c>
+      <c r="L71" t="inlineStr"/>
+      <c r="M71" t="inlineStr"/>
       <c r="N71" t="inlineStr"/>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Tackling climate change with data science and AI</t>
+          <t>Modelling deep convection and its impacts on the tropical tropopause layer</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
         <is>
-          <t>techreport</t>
-        </is>
-      </c>
-      <c r="Q71" t="inlineStr">
-        <is>
-          <t>https://doi.org/10.5281/zenodo.7712969</t>
-        </is>
-      </c>
-      <c r="R71" t="inlineStr"/>
+          <t>article</t>
+        </is>
+      </c>
+      <c r="Q71" t="inlineStr"/>
+      <c r="R71" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
       <c r="S71" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>2010</t>
         </is>
       </c>
     </row>
@@ -4440,32 +4444,44 @@
       <c r="A72" t="inlineStr"/>
       <c r="B72" t="inlineStr">
         <is>
-          <t>D. J. Patterson et al.</t>
-        </is>
-      </c>
-      <c r="C72" t="inlineStr"/>
+          <t>A. Conner, S. Hosking, J. Lloyd, A. Rao, G. Shaddick, M. Sharan</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>10.5281/zenodo.7712969</t>
+        </is>
+      </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>WWF and World Bank Group</t>
+          <t>The Alan Turing Institute</t>
         </is>
       </c>
       <c r="E72" t="inlineStr"/>
       <c r="F72" t="inlineStr"/>
       <c r="G72" t="inlineStr"/>
       <c r="H72" t="inlineStr"/>
-      <c r="I72" t="inlineStr"/>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>March</t>
+        </is>
+      </c>
       <c r="J72" t="inlineStr"/>
       <c r="K72" t="inlineStr"/>
       <c r="L72" t="inlineStr">
         <is>
-          <t>https://www.wwf.org.uk/sites/default/files/2020-12/Spatial%20Finance_%20Challenges%20and%20Opportunities_Final.pdf</t>
-        </is>
-      </c>
-      <c r="M72" t="inlineStr"/>
+          <t>https://zenodo.org/record/7712969/files/turing_asg_whitepaper_climatechange.pdf</t>
+        </is>
+      </c>
+      <c r="M72" t="inlineStr">
+        <is>
+          <t>Zenodo</t>
+        </is>
+      </c>
       <c r="N72" t="inlineStr"/>
       <c r="O72" t="inlineStr">
         <is>
-          <t>Spatial Finance: Challenges and Opportunities in a Changing World</t>
+          <t>Tackling climate change with data science and AI</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
@@ -4473,11 +4489,15 @@
           <t>techreport</t>
         </is>
       </c>
-      <c r="Q72" t="inlineStr"/>
+      <c r="Q72" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.5281/zenodo.7712969</t>
+        </is>
+      </c>
       <c r="R72" t="inlineStr"/>
       <c r="S72" t="inlineStr">
         <is>
-          <t>2020</t>
+          <t>2023</t>
         </is>
       </c>
     </row>
@@ -4485,13 +4505,13 @@
       <c r="A73" t="inlineStr"/>
       <c r="B73" t="inlineStr">
         <is>
-          <t>E. Wolff et al.</t>
+          <t>D. J. Patterson et al.</t>
         </is>
       </c>
       <c r="C73" t="inlineStr"/>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Global Environmental Research Committee (GERC), Royal Society</t>
+          <t>WWF and World Bank Group</t>
         </is>
       </c>
       <c r="E73" t="inlineStr"/>
@@ -4503,14 +4523,14 @@
       <c r="K73" t="inlineStr"/>
       <c r="L73" t="inlineStr">
         <is>
-          <t>https://royalsociety.org/-/media/policy/topics/energy-environment-climate/gerc-geoengineering-report.pdf</t>
+          <t>https://www.wwf.org.uk/sites/default/files/2020-12/Spatial%20Finance_%20Challenges%20and%20Opportunities_Final.pdf</t>
         </is>
       </c>
       <c r="M73" t="inlineStr"/>
       <c r="N73" t="inlineStr"/>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Geoengineering</t>
+          <t>Spatial Finance: Challenges and Opportunities in a Changing World</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
@@ -4522,7 +4542,7 @@
       <c r="R73" t="inlineStr"/>
       <c r="S73" t="inlineStr">
         <is>
-          <t>2018</t>
+          <t>2020</t>
         </is>
       </c>
     </row>
@@ -4548,14 +4568,14 @@
       <c r="K74" t="inlineStr"/>
       <c r="L74" t="inlineStr">
         <is>
-          <t>https://royalsociety.org/-/media/policy/topics/energy-environment-climate/gerc-air-quality-report.pdf</t>
+          <t>https://royalsociety.org/-/media/policy/topics/energy-environment-climate/gerc-geoengineering-report.pdf</t>
         </is>
       </c>
       <c r="M74" t="inlineStr"/>
       <c r="N74" t="inlineStr"/>
       <c r="O74" t="inlineStr">
         <is>
-          <t>Air quality</t>
+          <t>Geoengineering</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
@@ -4567,7 +4587,7 @@
       <c r="R74" t="inlineStr"/>
       <c r="S74" t="inlineStr">
         <is>
-          <t>2017</t>
+          <t>2018</t>
         </is>
       </c>
     </row>
@@ -4593,14 +4613,14 @@
       <c r="K75" t="inlineStr"/>
       <c r="L75" t="inlineStr">
         <is>
-          <t>https://royalsociety.org/-/media/policy/topics/energy-environment-climate/gerc-biodiversity-report.pdf</t>
+          <t>https://royalsociety.org/-/media/policy/topics/energy-environment-climate/gerc-air-quality-report.pdf</t>
         </is>
       </c>
       <c r="M75" t="inlineStr"/>
       <c r="N75" t="inlineStr"/>
       <c r="O75" t="inlineStr">
         <is>
-          <t>Biodiversity</t>
+          <t>Air quality</t>
         </is>
       </c>
       <c r="P75" t="inlineStr">
@@ -4638,14 +4658,14 @@
       <c r="K76" t="inlineStr"/>
       <c r="L76" t="inlineStr">
         <is>
-          <t>https://royalsociety.org/-/media/policy/topics/energy-environment-climate/gerc-naturalres-food-report.pdf?la=en-GB&amp;hash=54A9DBF67437B62966A6CD8B425A5D17</t>
+          <t>https://royalsociety.org/-/media/policy/topics/energy-environment-climate/gerc-biodiversity-report.pdf</t>
         </is>
       </c>
       <c r="M76" t="inlineStr"/>
       <c r="N76" t="inlineStr"/>
       <c r="O76" t="inlineStr">
         <is>
-          <t>Natural Resources</t>
+          <t>Biodiversity</t>
         </is>
       </c>
       <c r="P76" t="inlineStr">
@@ -4657,7 +4677,7 @@
       <c r="R76" t="inlineStr"/>
       <c r="S76" t="inlineStr">
         <is>
-          <t>2016</t>
+          <t>2017</t>
         </is>
       </c>
     </row>
@@ -4683,14 +4703,14 @@
       <c r="K77" t="inlineStr"/>
       <c r="L77" t="inlineStr">
         <is>
-          <t>https://royalsociety.org/-/media/policy/topics/energy-environment-climate/gerc-climate-report.pdf</t>
+          <t>https://royalsociety.org/-/media/policy/topics/energy-environment-climate/gerc-naturalres-food-report.pdf?la=en-GB&amp;hash=54A9DBF67437B62966A6CD8B425A5D17</t>
         </is>
       </c>
       <c r="M77" t="inlineStr"/>
       <c r="N77" t="inlineStr"/>
       <c r="O77" t="inlineStr">
         <is>
-          <t>Climate</t>
+          <t>Natural Resources</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
@@ -4710,13 +4730,13 @@
       <c r="A78" t="inlineStr"/>
       <c r="B78" t="inlineStr">
         <is>
-          <t>A. Maycock, S. Hosking, T. Bracegirdle</t>
+          <t>E. Wolff et al.</t>
         </is>
       </c>
       <c r="C78" t="inlineStr"/>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Cambridge Centre for Climate Science (CCfCS)</t>
+          <t>Global Environmental Research Committee (GERC), Royal Society</t>
         </is>
       </c>
       <c r="E78" t="inlineStr"/>
@@ -4728,14 +4748,14 @@
       <c r="K78" t="inlineStr"/>
       <c r="L78" t="inlineStr">
         <is>
-          <t>https://www.climatescience.cam.ac.uk/docs/ccfcs-ipcc-key-points-pdf</t>
+          <t>https://royalsociety.org/-/media/policy/topics/energy-environment-climate/gerc-climate-report.pdf</t>
         </is>
       </c>
       <c r="M78" t="inlineStr"/>
       <c r="N78" t="inlineStr"/>
       <c r="O78" t="inlineStr">
         <is>
-          <t>Key Points from the IPCC WGI Fifth Assessment Report. Climate Change 2013: The Physical Science Basis</t>
+          <t>Climate</t>
         </is>
       </c>
       <c r="P78" t="inlineStr">
@@ -4747,65 +4767,61 @@
       <c r="R78" t="inlineStr"/>
       <c r="S78" t="inlineStr">
         <is>
-          <t>2013</t>
+          <t>2016</t>
         </is>
       </c>
     </row>
     <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>Cambridge, UK</t>
-        </is>
-      </c>
+      <c r="A79" t="inlineStr"/>
       <c r="B79" t="inlineStr">
         <is>
-          <t>J. S. Hosking</t>
+          <t>A. Maycock, S. Hosking, T. Bracegirdle</t>
         </is>
       </c>
       <c r="C79" t="inlineStr"/>
-      <c r="D79" t="inlineStr"/>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Cambridge Centre for Climate Science (CCfCS)</t>
+        </is>
+      </c>
       <c r="E79" t="inlineStr"/>
       <c r="F79" t="inlineStr"/>
       <c r="G79" t="inlineStr"/>
       <c r="H79" t="inlineStr"/>
-      <c r="I79" t="inlineStr">
-        <is>
-          <t>March</t>
-        </is>
-      </c>
+      <c r="I79" t="inlineStr"/>
       <c r="J79" t="inlineStr"/>
       <c r="K79" t="inlineStr"/>
-      <c r="L79" t="inlineStr"/>
+      <c r="L79" t="inlineStr">
+        <is>
+          <t>https://www.climatescience.cam.ac.uk/docs/ccfcs-ipcc-key-points-pdf</t>
+        </is>
+      </c>
       <c r="M79" t="inlineStr"/>
-      <c r="N79" t="inlineStr">
-        <is>
-          <t>University of Cambridge</t>
-        </is>
-      </c>
+      <c r="N79" t="inlineStr"/>
       <c r="O79" t="inlineStr">
         <is>
-          <t>The impact of deep convection on the structure of, and transport through, the tropical tropopause layer</t>
+          <t>Key Points from the IPCC WGI Fifth Assessment Report. Climate Change 2013: The Physical Science Basis</t>
         </is>
       </c>
       <c r="P79" t="inlineStr">
         <is>
-          <t>phdthesis</t>
-        </is>
-      </c>
-      <c r="Q79" t="inlineStr">
-        <is>
-          <t>http://ethos.bl.uk/OrderDetails.do?uin=uk.bl.ethos.604249</t>
-        </is>
-      </c>
+          <t>techreport</t>
+        </is>
+      </c>
+      <c r="Q79" t="inlineStr"/>
       <c r="R79" t="inlineStr"/>
       <c r="S79" t="inlineStr">
         <is>
-          <t>2010</t>
+          <t>2013</t>
         </is>
       </c>
     </row>
     <row r="80">
-      <c r="A80" t="inlineStr"/>
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Cambridge, UK</t>
+        </is>
+      </c>
       <c r="B80" t="inlineStr">
         <is>
           <t>J. S. Hosking</t>
@@ -4817,35 +4833,47 @@
       <c r="F80" t="inlineStr"/>
       <c r="G80" t="inlineStr"/>
       <c r="H80" t="inlineStr"/>
-      <c r="I80" t="inlineStr"/>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>March</t>
+        </is>
+      </c>
       <c r="J80" t="inlineStr"/>
       <c r="K80" t="inlineStr"/>
       <c r="L80" t="inlineStr"/>
       <c r="M80" t="inlineStr"/>
-      <c r="N80" t="inlineStr"/>
+      <c r="N80" t="inlineStr">
+        <is>
+          <t>University of Cambridge</t>
+        </is>
+      </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>Amundsen Sea Low (ASL) index</t>
+          <t>The impact of deep convection on the structure of, and transport through, the tropical tropopause layer</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
         <is>
-          <t>datasets</t>
+          <t>phdthesis</t>
         </is>
       </c>
       <c r="Q80" t="inlineStr">
         <is>
-          <t>https://scotthosking.com/asl_index</t>
+          <t>http://ethos.bl.uk/OrderDetails.do?uin=uk.bl.ethos.604249</t>
         </is>
       </c>
       <c r="R80" t="inlineStr"/>
-      <c r="S80" t="inlineStr"/>
+      <c r="S80" t="inlineStr">
+        <is>
+          <t>2010</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr"/>
       <c r="B81" t="inlineStr">
         <is>
-          <t>T. Andersson, J. S. Hosking et al.</t>
+          <t>J. S. Hosking</t>
         </is>
       </c>
       <c r="C81" t="inlineStr"/>
@@ -4862,7 +4890,7 @@
       <c r="N81" t="inlineStr"/>
       <c r="O81" t="inlineStr">
         <is>
-          <t>Forecasts, neural networks, and results from the paper: 'Seasonal Arctic sea ice forecasting with probabilistic deep learning'</t>
+          <t>Amundsen Sea Low (ASL) index</t>
         </is>
       </c>
       <c r="P81" t="inlineStr">
@@ -4872,11 +4900,48 @@
       </c>
       <c r="Q81" t="inlineStr">
         <is>
-          <t>https://data.bas.ac.uk/full-record.php?id=GB/NERC/BAS/PDC/01526</t>
+          <t>https://scotthosking.com/asl_index</t>
         </is>
       </c>
       <c r="R81" t="inlineStr"/>
       <c r="S81" t="inlineStr"/>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr"/>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>T. Andersson, J. S. Hosking et al.</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr"/>
+      <c r="D82" t="inlineStr"/>
+      <c r="E82" t="inlineStr"/>
+      <c r="F82" t="inlineStr"/>
+      <c r="G82" t="inlineStr"/>
+      <c r="H82" t="inlineStr"/>
+      <c r="I82" t="inlineStr"/>
+      <c r="J82" t="inlineStr"/>
+      <c r="K82" t="inlineStr"/>
+      <c r="L82" t="inlineStr"/>
+      <c r="M82" t="inlineStr"/>
+      <c r="N82" t="inlineStr"/>
+      <c r="O82" t="inlineStr">
+        <is>
+          <t>Forecasts, neural networks, and results from the paper: 'Seasonal Arctic sea ice forecasting with probabilistic deep learning'</t>
+        </is>
+      </c>
+      <c r="P82" t="inlineStr">
+        <is>
+          <t>datasets</t>
+        </is>
+      </c>
+      <c r="Q82" t="inlineStr">
+        <is>
+          <t>https://data.bas.ac.uk/full-record.php?id=GB/NERC/BAS/PDC/01526</t>
+        </is>
+      </c>
+      <c r="R82" t="inlineStr"/>
+      <c r="S82" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>